<commit_message>
Desktop: added some logs
</commit_message>
<xml_diff>
--- a/logs/recap risultati.xlsx
+++ b/logs/recap risultati.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mp95\PycharmProjects\Thesis\logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC586847-FA7C-4F3E-A265-47287309CDB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AA1F0C6-0CA5-45B4-BC53-947B97BC01AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -121,10 +121,10 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -406,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -420,8 +420,8 @@
     <col min="9" max="9" width="24.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C1" t="s">
@@ -436,7 +436,7 @@
       <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="J1" t="s">
@@ -453,7 +453,7 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
+      <c r="A2" s="2"/>
       <c r="B2" t="s">
         <v>4</v>
       </c>
@@ -470,24 +470,9 @@
         <v>0.02</v>
       </c>
       <c r="H2" s="1"/>
-      <c r="I2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J2">
-        <v>0.99</v>
-      </c>
-      <c r="K2">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="L2">
-        <v>0.73</v>
-      </c>
-      <c r="M2">
-        <v>0.02</v>
-      </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
+      <c r="A3" s="2"/>
       <c r="B3" t="s">
         <v>5</v>
       </c>
@@ -504,24 +489,9 @@
         <v>0.04</v>
       </c>
       <c r="H3" s="1"/>
-      <c r="I3" t="s">
-        <v>11</v>
-      </c>
-      <c r="J3">
-        <v>0.99</v>
-      </c>
-      <c r="K3">
-        <v>9.0999999999999998E-2</v>
-      </c>
-      <c r="L3">
-        <v>0.73299999999999998</v>
-      </c>
-      <c r="M3">
-        <v>1.4E-2</v>
-      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
+      <c r="A4" s="2"/>
       <c r="B4" t="s">
         <v>6</v>
       </c>
@@ -538,63 +508,15 @@
         <v>0.01</v>
       </c>
       <c r="H4" s="1"/>
-      <c r="I4" t="s">
-        <v>12</v>
-      </c>
-      <c r="J4">
-        <v>0.97</v>
-      </c>
-      <c r="K4">
-        <v>7.9000000000000001E-2</v>
-      </c>
-      <c r="L4">
-        <v>0.72799999999999998</v>
-      </c>
-      <c r="M4">
-        <v>1.6E-2</v>
-      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="H5" s="1"/>
-      <c r="I5" t="s">
-        <v>13</v>
-      </c>
-      <c r="J5">
-        <v>0.97</v>
-      </c>
-      <c r="K5">
-        <v>7.5999999999999998E-2</v>
-      </c>
-      <c r="L5">
-        <v>0.73199999999999998</v>
-      </c>
-      <c r="M5">
-        <v>1.4E-2</v>
-      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="H6" s="1"/>
-      <c r="I6" t="s">
-        <v>14</v>
-      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="H7" s="1"/>
-      <c r="I7" t="s">
-        <v>15</v>
-      </c>
-      <c r="J7">
-        <v>0.97</v>
-      </c>
-      <c r="K7">
-        <v>9.1999999999999998E-2</v>
-      </c>
-      <c r="L7">
-        <v>0.72799999999999998</v>
-      </c>
-      <c r="M7">
-        <v>1.6799999999999999E-2</v>
-      </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="H8" s="1"/>
@@ -608,10 +530,130 @@
       </c>
       <c r="H10" s="1"/>
     </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H11" s="1"/>
+      <c r="I11" t="s">
+        <v>10</v>
+      </c>
+      <c r="J11">
+        <v>0.99</v>
+      </c>
+      <c r="K11">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="L11">
+        <v>0.73</v>
+      </c>
+      <c r="M11">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H12" s="1"/>
+      <c r="I12" t="s">
+        <v>11</v>
+      </c>
+      <c r="J12">
+        <v>0.99</v>
+      </c>
+      <c r="K12">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="L12">
+        <v>0.73299999999999998</v>
+      </c>
+      <c r="M12">
+        <v>1.4E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H13" s="1"/>
+      <c r="I13" t="s">
+        <v>12</v>
+      </c>
+      <c r="J13">
+        <v>0.97</v>
+      </c>
+      <c r="K13">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="L13">
+        <v>0.72799999999999998</v>
+      </c>
+      <c r="M13">
+        <v>1.6E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H14" s="1"/>
+      <c r="I14" t="s">
+        <v>13</v>
+      </c>
+      <c r="J14">
+        <v>0.97</v>
+      </c>
+      <c r="K14">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="L14">
+        <v>0.73199999999999998</v>
+      </c>
+      <c r="M14">
+        <v>1.4E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H15" s="1"/>
+      <c r="I15" t="s">
+        <v>14</v>
+      </c>
+      <c r="J15">
+        <v>1.04</v>
+      </c>
+      <c r="K15">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="L15">
+        <v>0.71199999999999997</v>
+      </c>
+      <c r="M15">
+        <v>1.2999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H16" s="1"/>
+      <c r="I16" t="s">
+        <v>15</v>
+      </c>
+      <c r="J16">
+        <v>0.97</v>
+      </c>
+      <c r="K16">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="L16">
+        <v>0.72799999999999998</v>
+      </c>
+      <c r="M16">
+        <v>1.6799999999999999E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H19" s="1"/>
+    </row>
+    <row r="20" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H20" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:A4"/>
-    <mergeCell ref="H1:H10"/>
+    <mergeCell ref="H1:H20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Desktop: google colab test results for architecture selection
</commit_message>
<xml_diff>
--- a/logs/recap risultati.xlsx
+++ b/logs/recap risultati.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mp95\PycharmProjects\Thesis\logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AA1F0C6-0CA5-45B4-BC53-947B97BC01AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1260C801-0A5B-45A8-90D5-367794DE8C3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
+    <sheet name="google colab" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="98">
   <si>
     <t>LOSS</t>
   </si>
@@ -83,12 +84,261 @@
   </si>
   <si>
     <t>MFCC+DELTAS+FORMANTS</t>
+  </si>
+  <si>
+    <t>MFCC</t>
+  </si>
+  <si>
+    <t>LPCC</t>
+  </si>
+  <si>
+    <t>Formants</t>
+  </si>
+  <si>
+    <t>Intensity</t>
+  </si>
+  <si>
+    <t>Pitch</t>
+  </si>
+  <si>
+    <t>MFCC+DELTAS+INTENSITY</t>
+  </si>
+  <si>
+    <t>MFCC+DELTAS+PITCH</t>
+  </si>
+  <si>
+    <t>0.969</t>
+  </si>
+  <si>
+    <t>0.073</t>
+  </si>
+  <si>
+    <t>0.726</t>
+  </si>
+  <si>
+    <t>0.014</t>
+  </si>
+  <si>
+    <t>0.730</t>
+  </si>
+  <si>
+    <t>0.068</t>
+  </si>
+  <si>
+    <t>0.016</t>
+  </si>
+  <si>
+    <t>0.966</t>
+  </si>
+  <si>
+    <t>0.729</t>
+  </si>
+  <si>
+    <t>0.069</t>
+  </si>
+  <si>
+    <t>0.018</t>
+  </si>
+  <si>
+    <t>MFCC+FORMANTS+INTENSITY</t>
+  </si>
+  <si>
+    <t>0.976</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.972</t>
+  </si>
+  <si>
+    <t>MFCC+FORMANTS+PITCH</t>
+  </si>
+  <si>
+    <t>Accuracy</t>
+  </si>
+  <si>
+    <t>Accuracy Std</t>
+  </si>
+  <si>
+    <t>Architecture</t>
+  </si>
+  <si>
+    <t>LSTM(128)</t>
+  </si>
+  <si>
+    <t>LSTM(128) dense (32)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7217638275623323  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.018558675441056865 </t>
+  </si>
+  <si>
+    <t>LSTM(128,64)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7269350280761718  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.016553848117565113 </t>
+  </si>
+  <si>
+    <t>LSTM(128,64) dense (32)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7342186107635499  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.015164536701452524 </t>
+  </si>
+  <si>
+    <t>LSTM(128,64,32)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.716618083000183  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.016822628471018324 </t>
+  </si>
+  <si>
+    <t>LSTM(256)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7272344141006469  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.012389178262122423 </t>
+  </si>
+  <si>
+    <t>0.7237927980422973</t>
+  </si>
+  <si>
+    <t>0.016837290992899854</t>
+  </si>
+  <si>
+    <t>LSTM(128) dense (64)</t>
+  </si>
+  <si>
+    <t>LSTM(128,64) dense (64)</t>
+  </si>
+  <si>
+    <t>LSTM(256) dense(128)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7297655827999115 </t>
+  </si>
+  <si>
+    <t>0.016247214906838364</t>
+  </si>
+  <si>
+    <t>LSTM(256) dense(64)</t>
+  </si>
+  <si>
+    <t>LSTM(256) dense(32)</t>
+  </si>
+  <si>
+    <t>LSTM(256) dense(256)</t>
+  </si>
+  <si>
+    <t>LSTM(256,128)</t>
+  </si>
+  <si>
+    <t>LSTM(256,128) dense(128)</t>
+  </si>
+  <si>
+    <t>LSTM(256,128) dense(64)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7292765583992005  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.013961241676636326 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7343757677078248  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.014737030499085807 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7371088638305663  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.01492163302836669 </t>
+  </si>
+  <si>
+    <t>LSTM(256,128,64)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7196242296695711  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.014563606178633075 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7182633891105651  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.013644830338469536 </t>
+  </si>
+  <si>
+    <t>LSTM(256,128,64) dense(32)</t>
+  </si>
+  <si>
+    <t>LSTM(512)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.715766457557678  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.013190663156989748 </t>
+  </si>
+  <si>
+    <t>LSTM(128) dense (128)</t>
+  </si>
+  <si>
+    <t>0.7284837546348573</t>
+  </si>
+  <si>
+    <t>0.015568647833485112</t>
+  </si>
+  <si>
+    <t>0.7138191375732422</t>
+  </si>
+  <si>
+    <t>0.01729179157499015</t>
+  </si>
+  <si>
+    <t>0.738351185798645</t>
+  </si>
+  <si>
+    <t>0.012935254446894239</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7360561892986296 </t>
+  </si>
+  <si>
+    <t>0.015110190517842797</t>
+  </si>
+  <si>
+    <t>0.7325092165470123</t>
+  </si>
+  <si>
+    <t>0.01461258374853887</t>
+  </si>
+  <si>
+    <t>0.7375539922714234</t>
+  </si>
+  <si>
+    <t>0.015035991166914243</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="167" formatCode="0.00000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -118,14 +368,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -408,8 +660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -421,7 +673,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C1" t="s">
@@ -436,7 +688,7 @@
       <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>9</v>
       </c>
       <c r="J1" t="s">
@@ -453,7 +705,7 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
+      <c r="A2" s="3"/>
       <c r="B2" t="s">
         <v>4</v>
       </c>
@@ -469,10 +721,25 @@
       <c r="F2">
         <v>0.02</v>
       </c>
-      <c r="H2" s="1"/>
+      <c r="H2" s="2"/>
+      <c r="I2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2">
+        <v>0.95</v>
+      </c>
+      <c r="K2">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="L2">
+        <v>0.70499999999999996</v>
+      </c>
+      <c r="M2">
+        <v>2.3E-2</v>
+      </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
+      <c r="A3" s="3"/>
       <c r="B3" t="s">
         <v>5</v>
       </c>
@@ -488,10 +755,19 @@
       <c r="F3">
         <v>0.04</v>
       </c>
-      <c r="H3" s="1"/>
+      <c r="H3" s="2"/>
+      <c r="I3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L3">
+        <v>0.51400000000000001</v>
+      </c>
+      <c r="M3">
+        <v>4.2000000000000003E-2</v>
+      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
+      <c r="A4" s="3"/>
       <c r="B4" t="s">
         <v>6</v>
       </c>
@@ -507,148 +783,247 @@
       <c r="F4">
         <v>0.01</v>
       </c>
-      <c r="H4" s="1"/>
+      <c r="H4" s="2"/>
+      <c r="I4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L4">
+        <v>0.253</v>
+      </c>
+      <c r="M4">
+        <v>1E-3</v>
+      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H5" s="1"/>
+      <c r="H5" s="2"/>
+      <c r="I5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5">
+        <v>1.08</v>
+      </c>
+      <c r="L5">
+        <v>0.253</v>
+      </c>
+      <c r="M5">
+        <v>1E-3</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H6" s="1"/>
+      <c r="H6" s="2"/>
+      <c r="I6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6">
+        <v>1.38</v>
+      </c>
+      <c r="L6">
+        <v>0.253</v>
+      </c>
+      <c r="M6">
+        <v>1E-3</v>
+      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H7" s="1"/>
+      <c r="H7" s="2"/>
+      <c r="I7" t="s">
+        <v>10</v>
+      </c>
+      <c r="J7">
+        <v>0.99</v>
+      </c>
+      <c r="K7">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="L7">
+        <v>0.73</v>
+      </c>
+      <c r="M7">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H8" s="1"/>
+      <c r="H8" s="2"/>
+      <c r="I8" t="s">
+        <v>11</v>
+      </c>
+      <c r="J8">
+        <v>0.99</v>
+      </c>
+      <c r="K8">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="L8">
+        <v>0.73299999999999998</v>
+      </c>
+      <c r="M8">
+        <v>1.4E-2</v>
+      </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H9" s="1"/>
+      <c r="H9" s="2"/>
+      <c r="I9" t="s">
+        <v>12</v>
+      </c>
+      <c r="J9">
+        <v>0.97</v>
+      </c>
+      <c r="K9">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="L9">
+        <v>0.72799999999999998</v>
+      </c>
+      <c r="M9">
+        <v>1.6E-2</v>
+      </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>8</v>
       </c>
-      <c r="H10" s="1"/>
+      <c r="H10" s="2"/>
+      <c r="I10" t="s">
+        <v>13</v>
+      </c>
+      <c r="J10">
+        <v>0.97</v>
+      </c>
+      <c r="K10">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="L10">
+        <v>0.73199999999999998</v>
+      </c>
+      <c r="M10">
+        <v>1.4E-2</v>
+      </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H11" s="1"/>
+      <c r="H11" s="2"/>
       <c r="I11" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="J11">
-        <v>0.99</v>
+        <v>1.04</v>
       </c>
       <c r="K11">
-        <v>7.0000000000000007E-2</v>
+        <v>8.7999999999999995E-2</v>
       </c>
       <c r="L11">
-        <v>0.73</v>
+        <v>0.71199999999999997</v>
       </c>
       <c r="M11">
-        <v>0.02</v>
+        <v>1.2999999999999999E-2</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H12" s="1"/>
+      <c r="H12" s="2"/>
       <c r="I12" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="J12">
-        <v>0.99</v>
+        <v>0.97</v>
       </c>
       <c r="K12">
-        <v>9.0999999999999998E-2</v>
+        <v>9.1999999999999998E-2</v>
       </c>
       <c r="L12">
-        <v>0.73299999999999998</v>
+        <v>0.72799999999999998</v>
       </c>
       <c r="M12">
-        <v>1.4E-2</v>
+        <v>1.6799999999999999E-2</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H13" s="1"/>
+      <c r="H13" s="2"/>
       <c r="I13" t="s">
-        <v>12</v>
-      </c>
-      <c r="J13">
-        <v>0.97</v>
-      </c>
-      <c r="K13">
-        <v>7.9000000000000001E-2</v>
-      </c>
-      <c r="L13">
-        <v>0.72799999999999998</v>
-      </c>
-      <c r="M13">
-        <v>1.6E-2</v>
+        <v>21</v>
+      </c>
+      <c r="J13" t="s">
+        <v>23</v>
+      </c>
+      <c r="K13" t="s">
+        <v>24</v>
+      </c>
+      <c r="L13" t="s">
+        <v>25</v>
+      </c>
+      <c r="M13" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H14" s="1"/>
+      <c r="H14" s="2"/>
       <c r="I14" t="s">
-        <v>13</v>
-      </c>
-      <c r="J14">
-        <v>0.97</v>
-      </c>
-      <c r="K14">
-        <v>7.5999999999999998E-2</v>
-      </c>
-      <c r="L14">
-        <v>0.73199999999999998</v>
-      </c>
-      <c r="M14">
-        <v>1.4E-2</v>
+        <v>15</v>
+      </c>
+      <c r="J14" s="1">
+        <v>1003</v>
+      </c>
+      <c r="K14" t="s">
+        <v>28</v>
+      </c>
+      <c r="L14" t="s">
+        <v>27</v>
+      </c>
+      <c r="M14" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H15" s="1"/>
+      <c r="H15" s="2"/>
       <c r="I15" t="s">
-        <v>14</v>
-      </c>
-      <c r="J15">
-        <v>1.04</v>
-      </c>
-      <c r="K15">
-        <v>8.7999999999999995E-2</v>
-      </c>
-      <c r="L15">
-        <v>0.71199999999999997</v>
-      </c>
-      <c r="M15">
-        <v>1.2999999999999999E-2</v>
+        <v>22</v>
+      </c>
+      <c r="J15" t="s">
+        <v>30</v>
+      </c>
+      <c r="K15" t="s">
+        <v>32</v>
+      </c>
+      <c r="L15" t="s">
+        <v>31</v>
+      </c>
+      <c r="M15" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H16" s="1"/>
+      <c r="H16" s="2"/>
       <c r="I16" t="s">
-        <v>15</v>
-      </c>
-      <c r="J16">
-        <v>0.97</v>
-      </c>
-      <c r="K16">
-        <v>9.1999999999999998E-2</v>
-      </c>
-      <c r="L16">
-        <v>0.72799999999999998</v>
-      </c>
-      <c r="M16">
-        <v>1.6799999999999999E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H17" s="1"/>
-    </row>
-    <row r="18" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H18" s="1"/>
-    </row>
-    <row r="19" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H19" s="1"/>
-    </row>
-    <row r="20" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H20" s="1"/>
+        <v>34</v>
+      </c>
+      <c r="J16" t="s">
+        <v>35</v>
+      </c>
+      <c r="K16" t="s">
+        <v>24</v>
+      </c>
+      <c r="L16" t="s">
+        <v>27</v>
+      </c>
+      <c r="M16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H17" s="2"/>
+      <c r="I17" t="s">
+        <v>37</v>
+      </c>
+      <c r="J17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H20" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -657,4 +1032,244 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E63792A-DA96-497B-A301-3EF736BC97C0}">
+  <dimension ref="A1:C20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" style="4" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>69</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>76</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>81</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>82</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Desktop: Added more parselmouth for parallel esecution, more logs
</commit_message>
<xml_diff>
--- a/logs/recap risultati.xlsx
+++ b/logs/recap risultati.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mp95\PycharmProjects\Thesis\logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1260C801-0A5B-45A8-90D5-367794DE8C3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87B055DA-193E-4DE7-AD7D-1DEEF86E9F11}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3660" yWindow="285" windowWidth="24930" windowHeight="15195" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
     <sheet name="google colab" sheetId="2" r:id="rId2"/>
+    <sheet name="setseed" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="133">
   <si>
     <t>LOSS</t>
   </si>
@@ -167,54 +168,18 @@
     <t>LSTM(128) dense (32)</t>
   </si>
   <si>
-    <t xml:space="preserve">0.7217638275623323  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.018558675441056865 </t>
-  </si>
-  <si>
     <t>LSTM(128,64)</t>
   </si>
   <si>
-    <t xml:space="preserve">0.7269350280761718  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.016553848117565113 </t>
-  </si>
-  <si>
     <t>LSTM(128,64) dense (32)</t>
   </si>
   <si>
-    <t xml:space="preserve">0.7342186107635499  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.015164536701452524 </t>
-  </si>
-  <si>
     <t>LSTM(128,64,32)</t>
   </si>
   <si>
-    <t xml:space="preserve">0.716618083000183  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.016822628471018324 </t>
-  </si>
-  <si>
     <t>LSTM(256)</t>
   </si>
   <si>
-    <t xml:space="preserve">0.7272344141006469  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.012389178262122423 </t>
-  </si>
-  <si>
-    <t>0.7237927980422973</t>
-  </si>
-  <si>
-    <t>0.016837290992899854</t>
-  </si>
-  <si>
     <t>LSTM(128) dense (64)</t>
   </si>
   <si>
@@ -224,12 +189,6 @@
     <t>LSTM(256) dense(128)</t>
   </si>
   <si>
-    <t xml:space="preserve">0.7297655827999115 </t>
-  </si>
-  <si>
-    <t>0.016247214906838364</t>
-  </si>
-  <si>
     <t>LSTM(256) dense(64)</t>
   </si>
   <si>
@@ -248,88 +207,235 @@
     <t>LSTM(256,128) dense(64)</t>
   </si>
   <si>
-    <t xml:space="preserve">0.7292765583992005  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.013961241676636326 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.7343757677078248  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.014737030499085807 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.7371088638305663  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.01492163302836669 </t>
-  </si>
-  <si>
     <t>LSTM(256,128,64)</t>
   </si>
   <si>
-    <t xml:space="preserve">0.7196242296695711  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.014563606178633075 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.7182633891105651  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.013644830338469536 </t>
-  </si>
-  <si>
     <t>LSTM(256,128,64) dense(32)</t>
   </si>
   <si>
     <t>LSTM(512)</t>
   </si>
   <si>
-    <t xml:space="preserve">0.715766457557678  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.013190663156989748 </t>
-  </si>
-  <si>
     <t>LSTM(128) dense (128)</t>
   </si>
   <si>
-    <t>0.7284837546348573</t>
-  </si>
-  <si>
-    <t>0.015568647833485112</t>
-  </si>
-  <si>
-    <t>0.7138191375732422</t>
-  </si>
-  <si>
-    <t>0.01729179157499015</t>
-  </si>
-  <si>
-    <t>0.738351185798645</t>
-  </si>
-  <si>
-    <t>0.012935254446894239</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.7360561892986296 </t>
-  </si>
-  <si>
-    <t>0.015110190517842797</t>
-  </si>
-  <si>
-    <t>0.7325092165470123</t>
-  </si>
-  <si>
-    <t>0.01461258374853887</t>
-  </si>
-  <si>
-    <t>0.7375539922714234</t>
-  </si>
-  <si>
-    <t>0.015035991166914243</t>
+    <t>TIME ELAPSED</t>
+  </si>
+  <si>
+    <t>TIME ELAPSED MINUTES</t>
+  </si>
+  <si>
+    <t>No dropout</t>
+  </si>
+  <si>
+    <t>0,711-0,017</t>
+  </si>
+  <si>
+    <t>0.734-0.013</t>
+  </si>
+  <si>
+    <t>LSTM(64)</t>
+  </si>
+  <si>
+    <t>0.6874451398849487</t>
+  </si>
+  <si>
+    <t>0.04559326591156529</t>
+  </si>
+  <si>
+    <t>0.7262071967124939</t>
+  </si>
+  <si>
+    <t>0.02903908374898274</t>
+  </si>
+  <si>
+    <t>0.042409243506034075</t>
+  </si>
+  <si>
+    <t>0.7082967400550843</t>
+  </si>
+  <si>
+    <t>0.024613515396868495</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7411325573921204 </t>
+  </si>
+  <si>
+    <t>0.6935469627380371</t>
+  </si>
+  <si>
+    <t>0.029601941834824324</t>
+  </si>
+  <si>
+    <t>0.6755926251411438</t>
+  </si>
+  <si>
+    <t>0.01974929808328549</t>
+  </si>
+  <si>
+    <t>0.6756365060806274</t>
+  </si>
+  <si>
+    <t>0.047235808541375886</t>
+  </si>
+  <si>
+    <t>0.7320895433425904</t>
+  </si>
+  <si>
+    <t>0.035665092169228814</t>
+  </si>
+  <si>
+    <t>0.6964003443717957</t>
+  </si>
+  <si>
+    <t>0.7172519564628601</t>
+  </si>
+  <si>
+    <t>0.036256365705922965</t>
+  </si>
+  <si>
+    <t>0.03274236925629052</t>
+  </si>
+  <si>
+    <t>0.708428430557251</t>
+  </si>
+  <si>
+    <t>0.05158689162013339</t>
+  </si>
+  <si>
+    <t>0.6962686538696289</t>
+  </si>
+  <si>
+    <t>0.04057396351040807</t>
+  </si>
+  <si>
+    <t>NO DROPOUTS</t>
+  </si>
+  <si>
+    <t>FULL DROPOUTS</t>
+  </si>
+  <si>
+    <t>0.7291922569274902</t>
+  </si>
+  <si>
+    <t>0.0343059053814798</t>
+  </si>
+  <si>
+    <t>0.7140474081039428</t>
+  </si>
+  <si>
+    <t>0.053803873106519705</t>
+  </si>
+  <si>
+    <t>0.7381035923957825</t>
+  </si>
+  <si>
+    <t>0.0306201469005738</t>
+  </si>
+  <si>
+    <t>0.6963564395904541</t>
+  </si>
+  <si>
+    <t>0.03273035916033609</t>
+  </si>
+  <si>
+    <t>0.6873573303222656</t>
+  </si>
+  <si>
+    <t>0.04202719778913188</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.7202809572219848</t>
+  </si>
+  <si>
+    <t>0.028447087748780485</t>
+  </si>
+  <si>
+    <t>0.7379719138145446</t>
+  </si>
+  <si>
+    <t>0.028620934249102448</t>
+  </si>
+  <si>
+    <t>0.038198853143585114</t>
+  </si>
+  <si>
+    <t>0.7202370524406433</t>
+  </si>
+  <si>
+    <t>NO DROPOUT LAST LAYER</t>
+  </si>
+  <si>
+    <t>0.708208954334259</t>
+  </si>
+  <si>
+    <t>0.04554074352595351</t>
+  </si>
+  <si>
+    <t>0.7171641826629639</t>
+  </si>
+  <si>
+    <t>0.042765819432748264</t>
+  </si>
+  <si>
+    <t>0.7262511014938354</t>
+  </si>
+  <si>
+    <t>0.03795156219124479</t>
+  </si>
+  <si>
+    <t>0.7172080755233765</t>
+  </si>
+  <si>
+    <t>0.010732709900697888</t>
+  </si>
+  <si>
+    <t>0.7260755181312561</t>
+  </si>
+  <si>
+    <t>0.7143985867500305</t>
+  </si>
+  <si>
+    <t>0.04380640425796567</t>
+  </si>
+  <si>
+    <t>0.03889198780827329</t>
+  </si>
+  <si>
+    <t>0.7261194109916687</t>
+  </si>
+  <si>
+    <t>0.043449853529563945</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7141791105270385 </t>
+  </si>
+  <si>
+    <t>0.028279541476297264</t>
+  </si>
+  <si>
+    <t>0.7410886645317077</t>
+  </si>
+  <si>
+    <t>0.029047708315010645</t>
+  </si>
+  <si>
+    <t>0.7231343269348145</t>
+  </si>
+  <si>
+    <t>0.02988801682690851</t>
+  </si>
+  <si>
+    <t>0.7142668962478638</t>
+  </si>
+  <si>
+    <t>0.029075175770494392</t>
+  </si>
+  <si>
+    <t>0.7320456624031066</t>
+  </si>
+  <si>
+    <t>0.039480620465651595</t>
   </si>
 </sst>
 </file>
@@ -337,7 +443,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.00000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -348,12 +454,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -368,16 +480,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -660,7 +779,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
@@ -673,7 +792,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C1" t="s">
@@ -688,7 +807,7 @@
       <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="7" t="s">
         <v>9</v>
       </c>
       <c r="J1" t="s">
@@ -705,7 +824,7 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
+      <c r="A2" s="8"/>
       <c r="B2" t="s">
         <v>4</v>
       </c>
@@ -721,7 +840,7 @@
       <c r="F2">
         <v>0.02</v>
       </c>
-      <c r="H2" s="2"/>
+      <c r="H2" s="7"/>
       <c r="I2" t="s">
         <v>16</v>
       </c>
@@ -739,7 +858,7 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
+      <c r="A3" s="8"/>
       <c r="B3" t="s">
         <v>5</v>
       </c>
@@ -755,7 +874,7 @@
       <c r="F3">
         <v>0.04</v>
       </c>
-      <c r="H3" s="2"/>
+      <c r="H3" s="7"/>
       <c r="I3" t="s">
         <v>17</v>
       </c>
@@ -767,7 +886,7 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
+      <c r="A4" s="8"/>
       <c r="B4" t="s">
         <v>6</v>
       </c>
@@ -783,7 +902,7 @@
       <c r="F4">
         <v>0.01</v>
       </c>
-      <c r="H4" s="2"/>
+      <c r="H4" s="7"/>
       <c r="I4" t="s">
         <v>18</v>
       </c>
@@ -795,7 +914,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H5" s="2"/>
+      <c r="H5" s="7"/>
       <c r="I5" t="s">
         <v>20</v>
       </c>
@@ -810,7 +929,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H6" s="2"/>
+      <c r="H6" s="7"/>
       <c r="I6" t="s">
         <v>19</v>
       </c>
@@ -825,7 +944,7 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H7" s="2"/>
+      <c r="H7" s="7"/>
       <c r="I7" t="s">
         <v>10</v>
       </c>
@@ -843,7 +962,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H8" s="2"/>
+      <c r="H8" s="7"/>
       <c r="I8" t="s">
         <v>11</v>
       </c>
@@ -861,7 +980,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H9" s="2"/>
+      <c r="H9" s="7"/>
       <c r="I9" t="s">
         <v>12</v>
       </c>
@@ -882,7 +1001,7 @@
       <c r="B10" t="s">
         <v>8</v>
       </c>
-      <c r="H10" s="2"/>
+      <c r="H10" s="7"/>
       <c r="I10" t="s">
         <v>13</v>
       </c>
@@ -900,7 +1019,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H11" s="2"/>
+      <c r="H11" s="7"/>
       <c r="I11" t="s">
         <v>14</v>
       </c>
@@ -918,7 +1037,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H12" s="2"/>
+      <c r="H12" s="7"/>
       <c r="I12" t="s">
         <v>15</v>
       </c>
@@ -936,7 +1055,7 @@
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H13" s="2"/>
+      <c r="H13" s="7"/>
       <c r="I13" t="s">
         <v>21</v>
       </c>
@@ -954,7 +1073,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H14" s="2"/>
+      <c r="H14" s="7"/>
       <c r="I14" t="s">
         <v>15</v>
       </c>
@@ -972,7 +1091,7 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H15" s="2"/>
+      <c r="H15" s="7"/>
       <c r="I15" t="s">
         <v>22</v>
       </c>
@@ -990,7 +1109,7 @@
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H16" s="2"/>
+      <c r="H16" s="7"/>
       <c r="I16" t="s">
         <v>34</v>
       </c>
@@ -1008,7 +1127,7 @@
       </c>
     </row>
     <row r="17" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H17" s="2"/>
+      <c r="H17" s="7"/>
       <c r="I17" t="s">
         <v>37</v>
       </c>
@@ -1017,13 +1136,13 @@
       </c>
     </row>
     <row r="18" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H18" s="2"/>
+      <c r="H18" s="7"/>
     </row>
     <row r="19" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H19" s="2"/>
+      <c r="H19" s="7"/>
     </row>
     <row r="20" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H20" s="2"/>
+      <c r="H20" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1036,240 +1155,786 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E63792A-DA96-497B-A301-3EF736BC97C0}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="2">
+        <v>0.72176382756233204</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1.8558675441056799E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="2">
+        <v>0.72379279804229701</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1.6837290992899798E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.72976558279991099</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1.6247214906838298E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.72848375463485704</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1.55686478334851E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.72693502807617105</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1.6553848117565099E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.734218610763549</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1.51645367014525E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.713819137573242</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1.7291791574990101E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0.71661808300018304</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1.68226284710183E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0.72723441410064604</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1.2389178262122401E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="4">
+        <v>0.738351185798645</v>
+      </c>
+      <c r="C11" s="4">
+        <v>1.2935254446894201E-2</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E11" s="6">
+        <v>3344</v>
+      </c>
+      <c r="F11" s="6">
+        <f>E11/60</f>
+        <v>55.733333333333334</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="4">
+        <v>0.73605618929862904</v>
+      </c>
+      <c r="C12" s="4">
+        <v>1.51101905178427E-2</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="6">
+        <v>3438</v>
+      </c>
+      <c r="F12" s="6">
+        <f t="shared" ref="F12:F17" si="0">E12/60</f>
+        <v>57.3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="2">
+        <v>0.73250921654701195</v>
+      </c>
+      <c r="C13" s="2">
+        <v>1.4612583748538801E-2</v>
+      </c>
+      <c r="F13" s="6"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" s="2">
+        <v>0.72927655839920003</v>
+      </c>
+      <c r="C14" s="2">
+        <v>1.39612416766363E-2</v>
+      </c>
+      <c r="F14" s="6"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="2">
+        <v>0.73437576770782398</v>
+      </c>
+      <c r="C15" s="2">
+        <v>1.47370304990858E-2</v>
+      </c>
+      <c r="F15" s="6"/>
+    </row>
+    <row r="16" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" s="4">
+        <v>0.73755399227142304</v>
+      </c>
+      <c r="C16" s="4">
+        <v>1.50359911669142E-2</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E16" s="6">
+        <v>5411</v>
+      </c>
+      <c r="F16" s="6">
+        <f t="shared" si="0"/>
+        <v>90.183333333333337</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" s="4">
+        <v>0.73710886383056595</v>
+      </c>
+      <c r="C17" s="4">
+        <v>1.4921633028366601E-2</v>
+      </c>
+      <c r="D17" s="4"/>
+      <c r="E17" s="6">
+        <v>5473</v>
+      </c>
+      <c r="F17" s="6">
+        <f t="shared" si="0"/>
+        <v>91.216666666666669</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" s="2">
+        <v>0.71962422966957096</v>
+      </c>
+      <c r="C18" s="2">
+        <v>1.4563606178633001E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="B19" s="2">
+        <v>0.71826338911056498</v>
+      </c>
+      <c r="C19" s="2">
+        <v>1.3644830338469501E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>85</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>60</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>51</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>54</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>66</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>61</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>64</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>65</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>67</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>68</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>69</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>76</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>81</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>82</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>84</v>
+      <c r="B20" s="2">
+        <v>0.71576645755767798</v>
+      </c>
+      <c r="C20" s="2">
+        <v>1.3190663156989701E-2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCD13E4E-D9D3-4F94-A17A-F26032C39845}">
+  <dimension ref="A1:K22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="19.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="E1" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="I1" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F3" t="s">
+        <v>100</v>
+      </c>
+      <c r="G3" t="s">
+        <v>101</v>
+      </c>
+      <c r="I3" t="s">
+        <v>65</v>
+      </c>
+      <c r="J3" t="s">
+        <v>66</v>
+      </c>
+      <c r="K3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" t="s">
+        <v>102</v>
+      </c>
+      <c r="G4" t="s">
+        <v>103</v>
+      </c>
+      <c r="I4" t="s">
+        <v>41</v>
+      </c>
+      <c r="J4" t="s">
+        <v>68</v>
+      </c>
+      <c r="K4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" t="s">
+        <v>109</v>
+      </c>
+      <c r="G5" t="s">
+        <v>110</v>
+      </c>
+      <c r="I5" t="s">
+        <v>42</v>
+      </c>
+      <c r="J5" t="s">
+        <v>117</v>
+      </c>
+      <c r="K5" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6" t="s">
+        <v>77</v>
+      </c>
+      <c r="E6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" t="s">
+        <v>111</v>
+      </c>
+      <c r="G6" t="s">
+        <v>112</v>
+      </c>
+      <c r="I6" t="s">
+        <v>47</v>
+      </c>
+      <c r="J6" t="s">
+        <v>123</v>
+      </c>
+      <c r="K6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" t="s">
+        <v>79</v>
+      </c>
+      <c r="E7" t="s">
+        <v>59</v>
+      </c>
+      <c r="F7" t="s">
+        <v>113</v>
+      </c>
+      <c r="G7" t="s">
+        <v>114</v>
+      </c>
+      <c r="I7" t="s">
+        <v>59</v>
+      </c>
+      <c r="J7" t="s">
+        <v>118</v>
+      </c>
+      <c r="K7" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8" t="s">
+        <v>81</v>
+      </c>
+      <c r="E8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" t="s">
+        <v>115</v>
+      </c>
+      <c r="G8" t="s">
+        <v>116</v>
+      </c>
+      <c r="I8" t="s">
+        <v>43</v>
+      </c>
+      <c r="J8" t="s">
+        <v>121</v>
+      </c>
+      <c r="K8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9" t="s">
+        <v>84</v>
+      </c>
+      <c r="E9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" t="s">
+        <v>92</v>
+      </c>
+      <c r="G9" t="s">
+        <v>93</v>
+      </c>
+      <c r="I9" t="s">
+        <v>44</v>
+      </c>
+      <c r="J9" t="s">
+        <v>125</v>
+      </c>
+      <c r="K9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" t="s">
+        <v>83</v>
+      </c>
+      <c r="C10" t="s">
+        <v>85</v>
+      </c>
+      <c r="E10" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" t="s">
+        <v>94</v>
+      </c>
+      <c r="G10" t="s">
+        <v>95</v>
+      </c>
+      <c r="I10" t="s">
+        <v>48</v>
+      </c>
+      <c r="J10" t="s">
+        <v>127</v>
+      </c>
+      <c r="K10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" t="s">
+        <v>88</v>
+      </c>
+      <c r="C11" t="s">
+        <v>89</v>
+      </c>
+      <c r="E11" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" t="s">
+        <v>98</v>
+      </c>
+      <c r="G11" t="s">
+        <v>99</v>
+      </c>
+      <c r="I11" t="s">
+        <v>45</v>
+      </c>
+      <c r="J11" t="s">
+        <v>129</v>
+      </c>
+      <c r="K11" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E12" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" t="s">
+        <v>104</v>
+      </c>
+      <c r="G12" t="s">
+        <v>105</v>
+      </c>
+      <c r="I12" t="s">
+        <v>46</v>
+      </c>
+      <c r="J12" t="s">
+        <v>73</v>
+      </c>
+      <c r="K12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" t="s">
+        <v>86</v>
+      </c>
+      <c r="C13" t="s">
+        <v>87</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F13" t="s">
+        <v>96</v>
+      </c>
+      <c r="G13" t="s">
+        <v>97</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="J13" t="s">
+        <v>131</v>
+      </c>
+      <c r="K13" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" t="s">
+        <v>50</v>
+      </c>
+      <c r="I15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" t="s">
+        <v>51</v>
+      </c>
+      <c r="I16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17" t="s">
+        <v>53</v>
+      </c>
+      <c r="I17" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>56</v>
+      </c>
+      <c r="E20" t="s">
+        <v>56</v>
+      </c>
+      <c r="I20" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>57</v>
+      </c>
+      <c r="E21" t="s">
+        <v>57</v>
+      </c>
+      <c r="I21" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" t="s">
+        <v>72</v>
+      </c>
+      <c r="E22" t="s">
+        <v>58</v>
+      </c>
+      <c r="F22" t="s">
+        <v>107</v>
+      </c>
+      <c r="G22" t="s">
+        <v>106</v>
+      </c>
+      <c r="I22" t="s">
+        <v>58</v>
+      </c>
+      <c r="J22" t="s">
+        <v>71</v>
+      </c>
+      <c r="K22" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="I1:K1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Desktop: added logs for 10 folder CV
</commit_message>
<xml_diff>
--- a/logs/recap risultati.xlsx
+++ b/logs/recap risultati.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mp95\PycharmProjects\Thesis\logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87B055DA-193E-4DE7-AD7D-1DEEF86E9F11}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F832D928-0BF2-43C7-9785-A938B6F6E05F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3660" yWindow="285" windowWidth="24930" windowHeight="15195" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="146">
   <si>
     <t>LOSS</t>
   </si>
@@ -436,6 +436,45 @@
   </si>
   <si>
     <t>0.039480620465651595</t>
+  </si>
+  <si>
+    <t>0.7203248381614685</t>
+  </si>
+  <si>
+    <t>0.026293621346120167</t>
+  </si>
+  <si>
+    <t>0.735030734539032</t>
+  </si>
+  <si>
+    <t>0.03248890475003557</t>
+  </si>
+  <si>
+    <t>0.051238683813622</t>
+  </si>
+  <si>
+    <t>0.726294994354248</t>
+  </si>
+  <si>
+    <t>0.05806351534832032</t>
+  </si>
+  <si>
+    <t>0.03157251168938171</t>
+  </si>
+  <si>
+    <t>0.035906858635031645</t>
+  </si>
+  <si>
+    <t>0.7290605902671814</t>
+  </si>
+  <si>
+    <t>0.029760749967404104</t>
+  </si>
+  <si>
+    <t>0.7559262394905091</t>
+  </si>
+  <si>
+    <t>0.012366525881863114</t>
   </si>
 </sst>
 </file>
@@ -1449,7 +1488,7 @@
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1819,8 +1858,20 @@
       <c r="E14" s="3" t="s">
         <v>49</v>
       </c>
+      <c r="F14" t="s">
+        <v>117</v>
+      </c>
+      <c r="G14" t="s">
+        <v>140</v>
+      </c>
       <c r="I14" s="3" t="s">
         <v>49</v>
+      </c>
+      <c r="J14" t="s">
+        <v>135</v>
+      </c>
+      <c r="K14" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -1830,8 +1881,20 @@
       <c r="E15" t="s">
         <v>50</v>
       </c>
+      <c r="F15" t="s">
+        <v>125</v>
+      </c>
+      <c r="G15" t="s">
+        <v>141</v>
+      </c>
       <c r="I15" t="s">
         <v>50</v>
+      </c>
+      <c r="J15" t="s">
+        <v>138</v>
+      </c>
+      <c r="K15" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -1841,8 +1904,20 @@
       <c r="E16" t="s">
         <v>51</v>
       </c>
+      <c r="F16" t="s">
+        <v>142</v>
+      </c>
+      <c r="G16" t="s">
+        <v>143</v>
+      </c>
       <c r="I16" t="s">
         <v>51</v>
+      </c>
+      <c r="J16" t="s">
+        <v>133</v>
+      </c>
+      <c r="K16" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -1852,8 +1927,20 @@
       <c r="E17" t="s">
         <v>53</v>
       </c>
+      <c r="F17" t="s">
+        <v>144</v>
+      </c>
+      <c r="G17" t="s">
+        <v>145</v>
+      </c>
       <c r="I17" t="s">
         <v>53</v>
+      </c>
+      <c r="J17" t="s">
+        <v>68</v>
+      </c>
+      <c r="K17" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Desktop: added xls results
</commit_message>
<xml_diff>
--- a/logs/recap risultati.xlsx
+++ b/logs/recap risultati.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mp95\PycharmProjects\Thesis\logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F832D928-0BF2-43C7-9785-A938B6F6E05F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{88D04BB0-1371-43F3-A89E-BE76FC451DD6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3660" yWindow="285" windowWidth="24930" windowHeight="15195" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3660" yWindow="285" windowWidth="24930" windowHeight="15195" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
     <sheet name="google colab" sheetId="2" r:id="rId2"/>
-    <sheet name="setseed" sheetId="3" r:id="rId3"/>
+    <sheet name="setseed5k" sheetId="3" r:id="rId3"/>
+    <sheet name="setseed10k" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="172">
   <si>
     <t>LOSS</t>
   </si>
@@ -237,244 +238,322 @@
     <t>LSTM(64)</t>
   </si>
   <si>
-    <t>0.6874451398849487</t>
-  </si>
-  <si>
-    <t>0.04559326591156529</t>
-  </si>
-  <si>
-    <t>0.7262071967124939</t>
-  </si>
-  <si>
-    <t>0.02903908374898274</t>
-  </si>
-  <si>
-    <t>0.042409243506034075</t>
-  </si>
-  <si>
-    <t>0.7082967400550843</t>
-  </si>
-  <si>
-    <t>0.024613515396868495</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.7411325573921204 </t>
-  </si>
-  <si>
-    <t>0.6935469627380371</t>
-  </si>
-  <si>
-    <t>0.029601941834824324</t>
-  </si>
-  <si>
-    <t>0.6755926251411438</t>
-  </si>
-  <si>
-    <t>0.01974929808328549</t>
-  </si>
-  <si>
-    <t>0.6756365060806274</t>
-  </si>
-  <si>
-    <t>0.047235808541375886</t>
-  </si>
-  <si>
-    <t>0.7320895433425904</t>
-  </si>
-  <si>
-    <t>0.035665092169228814</t>
-  </si>
-  <si>
-    <t>0.6964003443717957</t>
-  </si>
-  <si>
-    <t>0.7172519564628601</t>
-  </si>
-  <si>
-    <t>0.036256365705922965</t>
-  </si>
-  <si>
-    <t>0.03274236925629052</t>
-  </si>
-  <si>
-    <t>0.708428430557251</t>
-  </si>
-  <si>
-    <t>0.05158689162013339</t>
-  </si>
-  <si>
-    <t>0.6962686538696289</t>
-  </si>
-  <si>
-    <t>0.04057396351040807</t>
-  </si>
-  <si>
     <t>NO DROPOUTS</t>
   </si>
   <si>
     <t>FULL DROPOUTS</t>
   </si>
   <si>
-    <t>0.7291922569274902</t>
-  </si>
-  <si>
-    <t>0.0343059053814798</t>
-  </si>
-  <si>
-    <t>0.7140474081039428</t>
-  </si>
-  <si>
-    <t>0.053803873106519705</t>
-  </si>
-  <si>
-    <t>0.7381035923957825</t>
-  </si>
-  <si>
-    <t>0.0306201469005738</t>
-  </si>
-  <si>
-    <t>0.6963564395904541</t>
-  </si>
-  <si>
-    <t>0.03273035916033609</t>
-  </si>
-  <si>
-    <t>0.6873573303222656</t>
-  </si>
-  <si>
-    <t>0.04202719778913188</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.7202809572219848</t>
-  </si>
-  <si>
-    <t>0.028447087748780485</t>
-  </si>
-  <si>
-    <t>0.7379719138145446</t>
-  </si>
-  <si>
-    <t>0.028620934249102448</t>
-  </si>
-  <si>
-    <t>0.038198853143585114</t>
-  </si>
-  <si>
-    <t>0.7202370524406433</t>
-  </si>
-  <si>
     <t>NO DROPOUT LAST LAYER</t>
   </si>
   <si>
-    <t>0.708208954334259</t>
-  </si>
-  <si>
-    <t>0.04554074352595351</t>
-  </si>
-  <si>
-    <t>0.7171641826629639</t>
-  </si>
-  <si>
-    <t>0.042765819432748264</t>
-  </si>
-  <si>
-    <t>0.7262511014938354</t>
-  </si>
-  <si>
-    <t>0.03795156219124479</t>
-  </si>
-  <si>
-    <t>0.7172080755233765</t>
-  </si>
-  <si>
-    <t>0.010732709900697888</t>
-  </si>
-  <si>
-    <t>0.7260755181312561</t>
-  </si>
-  <si>
-    <t>0.7143985867500305</t>
-  </si>
-  <si>
-    <t>0.04380640425796567</t>
-  </si>
-  <si>
-    <t>0.03889198780827329</t>
-  </si>
-  <si>
-    <t>0.7261194109916687</t>
-  </si>
-  <si>
-    <t>0.043449853529563945</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.7141791105270385 </t>
-  </si>
-  <si>
-    <t>0.028279541476297264</t>
-  </si>
-  <si>
-    <t>0.7410886645317077</t>
-  </si>
-  <si>
-    <t>0.029047708315010645</t>
-  </si>
-  <si>
-    <t>0.7231343269348145</t>
-  </si>
-  <si>
-    <t>0.02988801682690851</t>
-  </si>
-  <si>
-    <t>0.7142668962478638</t>
-  </si>
-  <si>
-    <t>0.029075175770494392</t>
-  </si>
-  <si>
-    <t>0.7320456624031066</t>
-  </si>
-  <si>
-    <t>0.039480620465651595</t>
-  </si>
-  <si>
-    <t>0.7203248381614685</t>
-  </si>
-  <si>
-    <t>0.026293621346120167</t>
-  </si>
-  <si>
-    <t>0.735030734539032</t>
-  </si>
-  <si>
-    <t>0.03248890475003557</t>
-  </si>
-  <si>
-    <t>0.051238683813622</t>
-  </si>
-  <si>
-    <t>0.726294994354248</t>
-  </si>
-  <si>
-    <t>0.05806351534832032</t>
-  </si>
-  <si>
-    <t>0.03157251168938171</t>
-  </si>
-  <si>
-    <t>0.035906858635031645</t>
-  </si>
-  <si>
-    <t>0.7290605902671814</t>
-  </si>
-  <si>
-    <t>0.029760749967404104</t>
-  </si>
-  <si>
-    <t>0.7559262394905091</t>
-  </si>
-  <si>
-    <t>0.012366525881863114</t>
+    <t>0.7590017914772034</t>
+  </si>
+  <si>
+    <t>0.05325890896519597</t>
+  </si>
+  <si>
+    <t>0.7020499110221863</t>
+  </si>
+  <si>
+    <t>0.08021296184752935</t>
+  </si>
+  <si>
+    <t>0.7322638213634491</t>
+  </si>
+  <si>
+    <t>0.07093958903319733</t>
+  </si>
+  <si>
+    <t>0.7085561573505401</t>
+  </si>
+  <si>
+    <t>0.06344033394508111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.6787878781557083  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.10935882783927549  </t>
+  </si>
+  <si>
+    <t>0.759090918302536</t>
+  </si>
+  <si>
+    <t>0.06358173387784516</t>
+  </si>
+  <si>
+    <t>0.746880578994751</t>
+  </si>
+  <si>
+    <t>0.07654824535673742</t>
+  </si>
+  <si>
+    <t>0.7262032091617584</t>
+  </si>
+  <si>
+    <t>0.05915319035203717</t>
+  </si>
+  <si>
+    <t>0.7348484754562378</t>
+  </si>
+  <si>
+    <t>0.06652358182743892</t>
+  </si>
+  <si>
+    <t>0.7649732649326324</t>
+  </si>
+  <si>
+    <t>0.04590329043710351</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7352049887180329  </t>
+  </si>
+  <si>
+    <t>0.06336823291250288</t>
+  </si>
+  <si>
+    <t>0.762210339307785</t>
+  </si>
+  <si>
+    <t>0.07008408082386218</t>
+  </si>
+  <si>
+    <t>0.7501782596111297</t>
+  </si>
+  <si>
+    <t>0.04518646133903952</t>
+  </si>
+  <si>
+    <t>0.7681818187236786</t>
+  </si>
+  <si>
+    <t>0.051071077961338134</t>
+  </si>
+  <si>
+    <t>0.770944744348526</t>
+  </si>
+  <si>
+    <t>0.06314036835574521</t>
+  </si>
+  <si>
+    <t>0.061751001453896906</t>
+  </si>
+  <si>
+    <t>0.7737967908382416</t>
+  </si>
+  <si>
+    <t>0.042515891167034074</t>
+  </si>
+  <si>
+    <t>0.7708556115627289</t>
+  </si>
+  <si>
+    <t>0.09932510215261818</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7619429588317871  </t>
+  </si>
+  <si>
+    <t>0.7737967848777771</t>
+  </si>
+  <si>
+    <t>0.057730063506272536</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7474153339862823  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.07631564834152099  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7679144442081451  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.05218920974581887  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7677361845970154  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.06601287893824767  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.025823484551640637  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7766488373279572  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.031395325500609604  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7500891268253327  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.05590899343192252  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7381461679935455  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.06122001467009059  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7441176474094391  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0526291418700324  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7559714794158936  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.046944909503834946  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7769162237644196  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.04375206233526736  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7737967908382416  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.03795116810290435  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7799465298652649  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.07081771633972618  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7676470637321472  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.04047965276517804  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7679144382476807  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.04695404745223683  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7648841440677643  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.03825761552653673  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7706773757934571  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.05014594711373972  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7768270969390869  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.04195239738352049  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7975044548511505  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.04595819948864746  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7857397556304931  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.04729790924985195  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7827094554901123  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0324518693567599  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7855614960193634  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.04971983875716206  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7945632755756378  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.049141394508279125  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7796791553497314  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.04042416732337842  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7826203286647797  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.040691819639471216  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7707664906978607  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0402646941606926  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7884135544300079  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.03992073781479127  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7499108791351319  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.04467579656291825  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7675579369068146  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.053641751623085494  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.758734405040741  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.047598997655352665  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7796791434288025  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.04834045464414888  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7380570352077485  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.037007269917630786  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7707664966583252  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.050287915764755546  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7500000059604645  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.04596070609500026  </t>
   </si>
 </sst>
 </file>
@@ -519,7 +598,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -527,6 +606,12 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -831,7 +916,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C1" t="s">
@@ -846,7 +931,7 @@
       <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="9" t="s">
         <v>9</v>
       </c>
       <c r="J1" t="s">
@@ -863,7 +948,7 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
+      <c r="A2" s="10"/>
       <c r="B2" t="s">
         <v>4</v>
       </c>
@@ -879,7 +964,7 @@
       <c r="F2">
         <v>0.02</v>
       </c>
-      <c r="H2" s="7"/>
+      <c r="H2" s="9"/>
       <c r="I2" t="s">
         <v>16</v>
       </c>
@@ -897,7 +982,7 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
+      <c r="A3" s="10"/>
       <c r="B3" t="s">
         <v>5</v>
       </c>
@@ -913,7 +998,7 @@
       <c r="F3">
         <v>0.04</v>
       </c>
-      <c r="H3" s="7"/>
+      <c r="H3" s="9"/>
       <c r="I3" t="s">
         <v>17</v>
       </c>
@@ -925,7 +1010,7 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
+      <c r="A4" s="10"/>
       <c r="B4" t="s">
         <v>6</v>
       </c>
@@ -941,7 +1026,7 @@
       <c r="F4">
         <v>0.01</v>
       </c>
-      <c r="H4" s="7"/>
+      <c r="H4" s="9"/>
       <c r="I4" t="s">
         <v>18</v>
       </c>
@@ -953,7 +1038,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H5" s="7"/>
+      <c r="H5" s="9"/>
       <c r="I5" t="s">
         <v>20</v>
       </c>
@@ -968,7 +1053,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H6" s="7"/>
+      <c r="H6" s="9"/>
       <c r="I6" t="s">
         <v>19</v>
       </c>
@@ -983,7 +1068,7 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H7" s="7"/>
+      <c r="H7" s="9"/>
       <c r="I7" t="s">
         <v>10</v>
       </c>
@@ -1001,7 +1086,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H8" s="7"/>
+      <c r="H8" s="9"/>
       <c r="I8" t="s">
         <v>11</v>
       </c>
@@ -1019,7 +1104,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H9" s="7"/>
+      <c r="H9" s="9"/>
       <c r="I9" t="s">
         <v>12</v>
       </c>
@@ -1040,7 +1125,7 @@
       <c r="B10" t="s">
         <v>8</v>
       </c>
-      <c r="H10" s="7"/>
+      <c r="H10" s="9"/>
       <c r="I10" t="s">
         <v>13</v>
       </c>
@@ -1058,7 +1143,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H11" s="7"/>
+      <c r="H11" s="9"/>
       <c r="I11" t="s">
         <v>14</v>
       </c>
@@ -1076,7 +1161,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H12" s="7"/>
+      <c r="H12" s="9"/>
       <c r="I12" t="s">
         <v>15</v>
       </c>
@@ -1094,7 +1179,7 @@
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H13" s="7"/>
+      <c r="H13" s="9"/>
       <c r="I13" t="s">
         <v>21</v>
       </c>
@@ -1112,7 +1197,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H14" s="7"/>
+      <c r="H14" s="9"/>
       <c r="I14" t="s">
         <v>15</v>
       </c>
@@ -1130,7 +1215,7 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H15" s="7"/>
+      <c r="H15" s="9"/>
       <c r="I15" t="s">
         <v>22</v>
       </c>
@@ -1148,7 +1233,7 @@
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H16" s="7"/>
+      <c r="H16" s="9"/>
       <c r="I16" t="s">
         <v>34</v>
       </c>
@@ -1166,7 +1251,7 @@
       </c>
     </row>
     <row r="17" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H17" s="7"/>
+      <c r="H17" s="9"/>
       <c r="I17" t="s">
         <v>37</v>
       </c>
@@ -1175,13 +1260,13 @@
       </c>
     </row>
     <row r="18" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H18" s="7"/>
+      <c r="H18" s="9"/>
     </row>
     <row r="19" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H19" s="7"/>
+      <c r="H19" s="9"/>
     </row>
     <row r="20" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H20" s="7"/>
+      <c r="H20" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1485,10 +1570,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCD13E4E-D9D3-4F94-A17A-F26032C39845}">
-  <dimension ref="A1:K22"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1505,404 +1590,1054 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="E1" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="I1" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
+      <c r="A1" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="E1" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="I1" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I2" t="s">
-        <v>40</v>
-      </c>
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C3" t="s">
-        <v>67</v>
+        <v>40</v>
       </c>
       <c r="E3" t="s">
-        <v>65</v>
-      </c>
-      <c r="F3" t="s">
-        <v>100</v>
-      </c>
-      <c r="G3" t="s">
-        <v>101</v>
+        <v>40</v>
       </c>
       <c r="I3" t="s">
-        <v>65</v>
-      </c>
-      <c r="J3" t="s">
-        <v>66</v>
-      </c>
-      <c r="K3" t="s">
-        <v>67</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C4" t="s">
-        <v>69</v>
+        <v>65</v>
+      </c>
+      <c r="B4">
+        <v>0.68744513988494804</v>
+      </c>
+      <c r="C4">
+        <v>4.5593265911565199E-2</v>
       </c>
       <c r="E4" t="s">
-        <v>41</v>
-      </c>
-      <c r="F4" t="s">
-        <v>102</v>
-      </c>
-      <c r="G4" t="s">
-        <v>103</v>
+        <v>65</v>
+      </c>
+      <c r="F4">
+        <v>0.68735733032226498</v>
+      </c>
+      <c r="G4">
+        <v>4.2027197789131797E-2</v>
       </c>
       <c r="I4" t="s">
-        <v>41</v>
-      </c>
-      <c r="J4" t="s">
-        <v>68</v>
-      </c>
-      <c r="K4" t="s">
-        <v>69</v>
+        <v>65</v>
+      </c>
+      <c r="J4">
+        <v>0.68744513988494804</v>
+      </c>
+      <c r="K4">
+        <v>4.5593265911565199E-2</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B5" t="s">
-        <v>74</v>
-      </c>
-      <c r="C5" t="s">
-        <v>75</v>
+        <v>41</v>
+      </c>
+      <c r="B5">
+        <v>0.72620719671249301</v>
+      </c>
+      <c r="C5">
+        <v>2.9039083748982699E-2</v>
       </c>
       <c r="E5" t="s">
-        <v>42</v>
-      </c>
-      <c r="F5" t="s">
-        <v>109</v>
-      </c>
-      <c r="G5" t="s">
-        <v>110</v>
+        <v>41</v>
+      </c>
+      <c r="F5">
+        <v>0.72028095722198404</v>
+      </c>
+      <c r="G5">
+        <v>2.8447087748780402E-2</v>
       </c>
       <c r="I5" t="s">
-        <v>42</v>
-      </c>
-      <c r="J5" t="s">
-        <v>117</v>
-      </c>
-      <c r="K5" t="s">
-        <v>122</v>
+        <v>41</v>
+      </c>
+      <c r="J5">
+        <v>0.72620719671249301</v>
+      </c>
+      <c r="K5">
+        <v>2.9039083748982699E-2</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C6" t="s">
-        <v>77</v>
+        <v>42</v>
+      </c>
+      <c r="B6">
+        <v>0.69354696273803695</v>
+      </c>
+      <c r="C6">
+        <v>2.96019418348243E-2</v>
       </c>
       <c r="E6" t="s">
-        <v>47</v>
-      </c>
-      <c r="F6" t="s">
-        <v>111</v>
-      </c>
-      <c r="G6" t="s">
-        <v>112</v>
+        <v>42</v>
+      </c>
+      <c r="F6">
+        <v>0.70820895433425901</v>
+      </c>
+      <c r="G6">
+        <v>4.5540743525953498E-2</v>
       </c>
       <c r="I6" t="s">
-        <v>47</v>
-      </c>
-      <c r="J6" t="s">
-        <v>123</v>
-      </c>
-      <c r="K6" t="s">
-        <v>120</v>
+        <v>42</v>
+      </c>
+      <c r="J6">
+        <v>0.72607551813125604</v>
+      </c>
+      <c r="K6">
+        <v>4.3449853529563903E-2</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>59</v>
-      </c>
-      <c r="B7" t="s">
-        <v>78</v>
-      </c>
-      <c r="C7" t="s">
-        <v>79</v>
+        <v>47</v>
+      </c>
+      <c r="B7">
+        <v>0.67559262514114304</v>
+      </c>
+      <c r="C7">
+        <v>1.9749298083285401E-2</v>
       </c>
       <c r="E7" t="s">
-        <v>59</v>
-      </c>
-      <c r="F7" t="s">
-        <v>113</v>
-      </c>
-      <c r="G7" t="s">
-        <v>114</v>
+        <v>47</v>
+      </c>
+      <c r="F7">
+        <v>0.717164182662963</v>
+      </c>
+      <c r="G7">
+        <v>4.2765819432748202E-2</v>
       </c>
       <c r="I7" t="s">
-        <v>59</v>
-      </c>
-      <c r="J7" t="s">
-        <v>118</v>
-      </c>
-      <c r="K7" t="s">
-        <v>119</v>
+        <v>47</v>
+      </c>
+      <c r="J7">
+        <v>0.71417911052703797</v>
+      </c>
+      <c r="K7">
+        <v>3.8891987808273201E-2</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B8" t="s">
-        <v>80</v>
-      </c>
-      <c r="C8" t="s">
-        <v>81</v>
+        <v>59</v>
+      </c>
+      <c r="B8">
+        <v>0.67563650608062698</v>
+      </c>
+      <c r="C8">
+        <v>4.7235808541375802E-2</v>
       </c>
       <c r="E8" t="s">
-        <v>43</v>
-      </c>
-      <c r="F8" t="s">
-        <v>115</v>
-      </c>
-      <c r="G8" t="s">
-        <v>116</v>
+        <v>59</v>
+      </c>
+      <c r="F8">
+        <v>0.72625110149383498</v>
+      </c>
+      <c r="G8">
+        <v>3.7951562191244702E-2</v>
       </c>
       <c r="I8" t="s">
-        <v>43</v>
-      </c>
-      <c r="J8" t="s">
-        <v>121</v>
-      </c>
-      <c r="K8" t="s">
-        <v>124</v>
+        <v>59</v>
+      </c>
+      <c r="J8">
+        <v>0.71439858675002998</v>
+      </c>
+      <c r="K8">
+        <v>4.38064042579656E-2</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>44</v>
-      </c>
-      <c r="B9" t="s">
-        <v>82</v>
-      </c>
-      <c r="C9" t="s">
-        <v>84</v>
+        <v>43</v>
+      </c>
+      <c r="B9">
+        <v>0.73208954334259002</v>
+      </c>
+      <c r="C9">
+        <v>3.56650921692288E-2</v>
       </c>
       <c r="E9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F9" t="s">
-        <v>92</v>
-      </c>
-      <c r="G9" t="s">
-        <v>93</v>
+        <v>43</v>
+      </c>
+      <c r="F9">
+        <v>0.71720807552337595</v>
+      </c>
+      <c r="G9">
+        <v>1.0732709900697799E-2</v>
       </c>
       <c r="I9" t="s">
-        <v>44</v>
-      </c>
-      <c r="J9" t="s">
-        <v>125</v>
-      </c>
-      <c r="K9" t="s">
-        <v>126</v>
+        <v>43</v>
+      </c>
+      <c r="J9">
+        <v>0.72611941099166799</v>
+      </c>
+      <c r="K9">
+        <v>2.8279541476297201E-2</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>48</v>
-      </c>
-      <c r="B10" t="s">
-        <v>83</v>
-      </c>
-      <c r="C10" t="s">
-        <v>85</v>
+        <v>44</v>
+      </c>
+      <c r="B10">
+        <v>0.69640034437179499</v>
+      </c>
+      <c r="C10">
+        <v>3.6256365705922902E-2</v>
       </c>
       <c r="E10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F10" t="s">
-        <v>94</v>
-      </c>
-      <c r="G10" t="s">
-        <v>95</v>
+        <v>44</v>
+      </c>
+      <c r="F10">
+        <v>0.72919225692749001</v>
+      </c>
+      <c r="G10">
+        <v>3.4305905381479797E-2</v>
       </c>
       <c r="I10" t="s">
-        <v>48</v>
-      </c>
-      <c r="J10" t="s">
-        <v>127</v>
-      </c>
-      <c r="K10" t="s">
-        <v>128</v>
+        <v>44</v>
+      </c>
+      <c r="J10">
+        <v>0.74108866453170696</v>
+      </c>
+      <c r="K10">
+        <v>2.9047708315010599E-2</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>45</v>
-      </c>
-      <c r="B11" t="s">
-        <v>88</v>
-      </c>
-      <c r="C11" t="s">
-        <v>89</v>
+        <v>48</v>
+      </c>
+      <c r="B11">
+        <v>0.71725195646286</v>
+      </c>
+      <c r="C11">
+        <v>3.2742369256290503E-2</v>
       </c>
       <c r="E11" t="s">
-        <v>45</v>
-      </c>
-      <c r="F11" t="s">
-        <v>98</v>
-      </c>
-      <c r="G11" t="s">
-        <v>99</v>
+        <v>48</v>
+      </c>
+      <c r="F11">
+        <v>0.71404740810394196</v>
+      </c>
+      <c r="G11">
+        <v>5.3803873106519698E-2</v>
       </c>
       <c r="I11" t="s">
-        <v>45</v>
-      </c>
-      <c r="J11" t="s">
-        <v>129</v>
-      </c>
-      <c r="K11" t="s">
-        <v>130</v>
+        <v>48</v>
+      </c>
+      <c r="J11">
+        <v>0.72313432693481405</v>
+      </c>
+      <c r="K11">
+        <v>2.98880168269085E-2</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12">
+        <v>0.696268653869628</v>
+      </c>
+      <c r="C12">
+        <v>4.0573963510407998E-2</v>
+      </c>
+      <c r="E12" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12">
+        <v>0.69635643959045401</v>
+      </c>
+      <c r="G12">
+        <v>3.2730359160336002E-2</v>
+      </c>
+      <c r="I12" t="s">
+        <v>45</v>
+      </c>
+      <c r="J12">
+        <v>0.71426689624786299</v>
+      </c>
+      <c r="K12">
+        <v>2.9075175770494299E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>46</v>
       </c>
-      <c r="B12" t="s">
-        <v>73</v>
-      </c>
-      <c r="C12" t="s">
-        <v>70</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="B13">
+        <v>0.74113255739212003</v>
+      </c>
+      <c r="C13">
+        <v>4.2409243506033999E-2</v>
+      </c>
+      <c r="E13" t="s">
         <v>46</v>
       </c>
-      <c r="F12" t="s">
-        <v>104</v>
-      </c>
-      <c r="G12" t="s">
-        <v>105</v>
-      </c>
-      <c r="I12" t="s">
+      <c r="F13">
+        <v>0.73797191381454397</v>
+      </c>
+      <c r="G13">
+        <v>2.8620934249102399E-2</v>
+      </c>
+      <c r="I13" t="s">
         <v>46</v>
       </c>
-      <c r="J12" t="s">
-        <v>73</v>
-      </c>
-      <c r="K12" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="J13">
+        <v>0.74113255739212003</v>
+      </c>
+      <c r="K13">
+        <v>4.2409243506033999E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>52</v>
       </c>
-      <c r="B13" t="s">
-        <v>86</v>
-      </c>
-      <c r="C13" t="s">
-        <v>87</v>
-      </c>
-      <c r="E13" s="3" t="s">
+      <c r="B14">
+        <v>0.70842843055725102</v>
+      </c>
+      <c r="C14">
+        <v>5.1586891620133302E-2</v>
+      </c>
+      <c r="E14" t="s">
         <v>52</v>
       </c>
-      <c r="F13" t="s">
-        <v>96</v>
-      </c>
-      <c r="G13" t="s">
-        <v>97</v>
-      </c>
-      <c r="I13" s="3" t="s">
+      <c r="F14">
+        <v>0.73810359239578205</v>
+      </c>
+      <c r="G14">
+        <v>3.06201469005738E-2</v>
+      </c>
+      <c r="I14" t="s">
         <v>52</v>
       </c>
-      <c r="J13" t="s">
-        <v>131</v>
-      </c>
-      <c r="K13" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="F14" t="s">
-        <v>117</v>
-      </c>
-      <c r="G14" t="s">
-        <v>140</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="J14" t="s">
-        <v>135</v>
-      </c>
-      <c r="K14" t="s">
-        <v>136</v>
+      <c r="J14">
+        <v>0.73204566240310598</v>
+      </c>
+      <c r="K14">
+        <v>3.9480620465651498E-2</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>50</v>
+        <v>49</v>
+      </c>
+      <c r="B15">
+        <v>0.732133448123931</v>
+      </c>
+      <c r="C15">
+        <v>2.5024868500347301E-2</v>
       </c>
       <c r="E15" t="s">
-        <v>50</v>
-      </c>
-      <c r="F15" t="s">
-        <v>125</v>
-      </c>
-      <c r="G15" t="s">
-        <v>141</v>
+        <v>49</v>
+      </c>
+      <c r="F15">
+        <v>0.72607551813125604</v>
+      </c>
+      <c r="G15">
+        <v>3.1572511689381702E-2</v>
       </c>
       <c r="I15" t="s">
-        <v>50</v>
-      </c>
-      <c r="J15" t="s">
-        <v>138</v>
-      </c>
-      <c r="K15" t="s">
-        <v>139</v>
+        <v>49</v>
+      </c>
+      <c r="J15">
+        <v>0.735030734539032</v>
+      </c>
+      <c r="K15">
+        <v>3.2488904750035498E-2</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16">
+        <v>0.72032483816146797</v>
+      </c>
+      <c r="C16">
+        <v>2.6293621346120101E-2</v>
+      </c>
+      <c r="E16" t="s">
+        <v>50</v>
+      </c>
+      <c r="F16">
+        <v>0.74108866453170696</v>
+      </c>
+      <c r="G16">
+        <v>3.5906858635031597E-2</v>
+      </c>
+      <c r="I16" t="s">
+        <v>50</v>
+      </c>
+      <c r="J16">
+        <v>0.72629499435424805</v>
+      </c>
+      <c r="K16">
+        <v>5.8063515348320299E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>51</v>
       </c>
+      <c r="B17">
+        <v>0.71725196838378902</v>
+      </c>
+      <c r="C17">
+        <v>4.7227637451394099E-2</v>
+      </c>
+      <c r="E17" t="s">
+        <v>51</v>
+      </c>
+      <c r="F17">
+        <v>0.72906059026718095</v>
+      </c>
+      <c r="G17">
+        <v>2.9760749967404101E-2</v>
+      </c>
+      <c r="I17" t="s">
+        <v>51</v>
+      </c>
+      <c r="J17">
+        <v>0.72032483816146797</v>
+      </c>
+      <c r="K17">
+        <v>2.6293621346120101E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18">
+        <v>0.69942932128906199</v>
+      </c>
+      <c r="C18">
+        <v>2.34876090450012E-2</v>
+      </c>
+      <c r="E18" t="s">
+        <v>53</v>
+      </c>
+      <c r="F18">
+        <v>0.75592623949050897</v>
+      </c>
+      <c r="G18">
+        <v>1.23665258818631E-2</v>
+      </c>
+      <c r="I18" t="s">
+        <v>53</v>
+      </c>
+      <c r="J18">
+        <v>0.72620719671249301</v>
+      </c>
+      <c r="K18">
+        <v>5.1238683813622003E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19">
+        <v>0.72322212457656798</v>
+      </c>
+      <c r="C19">
+        <v>2.9124695929427399E-2</v>
+      </c>
+      <c r="E19" t="s">
+        <v>54</v>
+      </c>
+      <c r="F19">
+        <v>0.74100087881088195</v>
+      </c>
+      <c r="G19">
+        <v>2.66183628564154E-2</v>
+      </c>
+      <c r="I19" t="s">
+        <v>54</v>
+      </c>
+      <c r="J19">
+        <v>0.74407373666763299</v>
+      </c>
+      <c r="K19">
+        <v>2.53577887958517E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20">
+        <v>0.77080773115157997</v>
+      </c>
+      <c r="C20">
+        <v>2.7855240894788202E-2</v>
+      </c>
+      <c r="E20" t="s">
+        <v>55</v>
+      </c>
+      <c r="F20">
+        <v>0.72620719671249301</v>
+      </c>
+      <c r="G20">
+        <v>2.9039083748982699E-2</v>
+      </c>
+      <c r="I20" t="s">
+        <v>55</v>
+      </c>
+      <c r="J20">
+        <v>0.72914837598800597</v>
+      </c>
+      <c r="K20">
+        <v>2.7490199340737698E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21">
+        <v>0.68744512796401902</v>
+      </c>
+      <c r="C21">
+        <v>1.44050347752658E-2</v>
+      </c>
+      <c r="E21" t="s">
+        <v>56</v>
+      </c>
+      <c r="F21">
+        <v>0.70820895433425901</v>
+      </c>
+      <c r="G21">
+        <v>3.5665078450158601E-2</v>
+      </c>
+      <c r="I21" t="s">
+        <v>56</v>
+      </c>
+      <c r="J21">
+        <v>0.71413519382476798</v>
+      </c>
+      <c r="K21">
+        <v>4.7363162293743301E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22">
+        <v>0.74402984380722004</v>
+      </c>
+      <c r="C22">
+        <v>4.1657557452725001E-2</v>
+      </c>
+      <c r="E22" t="s">
+        <v>57</v>
+      </c>
+      <c r="F22">
+        <v>0.72313432693481405</v>
+      </c>
+      <c r="G22">
+        <v>3.6590005025564497E-2</v>
+      </c>
+      <c r="I22" t="s">
+        <v>57</v>
+      </c>
+      <c r="J22">
+        <v>0.72023705244064296</v>
+      </c>
+      <c r="K22">
+        <v>3.7014149298790301E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23">
+        <v>0.70829674005508403</v>
+      </c>
+      <c r="C23">
+        <v>2.4613515396868402E-2</v>
+      </c>
+      <c r="E23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F23">
+        <v>0.72023705244064296</v>
+      </c>
+      <c r="G23">
+        <v>3.81988531435851E-2</v>
+      </c>
+      <c r="I23" t="s">
+        <v>58</v>
+      </c>
+      <c r="J23">
+        <v>0.70829674005508403</v>
+      </c>
+      <c r="K23">
+        <v>2.4613515396868402E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="I1:K1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BED2715A-8FB0-46CE-8864-89EDF7D1B731}">
+  <dimension ref="A1:K22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:C22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="19.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="E1" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="I1" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" t="s">
+        <v>40</v>
+      </c>
+      <c r="I3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F4" t="s">
+        <v>77</v>
+      </c>
+      <c r="G4" t="s">
+        <v>78</v>
+      </c>
+      <c r="I4" t="s">
+        <v>65</v>
+      </c>
+      <c r="J4" t="s">
+        <v>71</v>
+      </c>
+      <c r="K4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" t="s">
+        <v>79</v>
+      </c>
+      <c r="G5" t="s">
+        <v>80</v>
+      </c>
+      <c r="I5" t="s">
+        <v>41</v>
+      </c>
+      <c r="J5" t="s">
+        <v>69</v>
+      </c>
+      <c r="K5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" t="s">
+        <v>74</v>
+      </c>
+      <c r="E6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" t="s">
+        <v>81</v>
+      </c>
+      <c r="G6" t="s">
+        <v>82</v>
+      </c>
+      <c r="I6" t="s">
+        <v>42</v>
+      </c>
+      <c r="J6" t="s">
+        <v>85</v>
+      </c>
+      <c r="K6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" t="s">
+        <v>83</v>
+      </c>
+      <c r="G7" t="s">
+        <v>84</v>
+      </c>
+      <c r="I7" t="s">
+        <v>47</v>
+      </c>
+      <c r="J7" t="s">
+        <v>87</v>
+      </c>
+      <c r="K7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C8" t="s">
+        <v>90</v>
+      </c>
+      <c r="E8" t="s">
+        <v>59</v>
+      </c>
+      <c r="F8" t="s">
+        <v>83</v>
+      </c>
+      <c r="G8" t="s">
+        <v>99</v>
+      </c>
+      <c r="I8" t="s">
+        <v>59</v>
+      </c>
+      <c r="J8" t="s">
+        <v>107</v>
+      </c>
+      <c r="K8" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C9" t="s">
+        <v>92</v>
+      </c>
+      <c r="E9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" t="s">
+        <v>97</v>
+      </c>
+      <c r="G9" t="s">
+        <v>98</v>
+      </c>
+      <c r="I9" t="s">
+        <v>43</v>
+      </c>
+      <c r="J9" t="s">
+        <v>105</v>
+      </c>
+      <c r="K9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" t="s">
+        <v>93</v>
+      </c>
+      <c r="C10" t="s">
+        <v>94</v>
+      </c>
+      <c r="E10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" t="s">
+        <v>100</v>
+      </c>
+      <c r="G10" t="s">
+        <v>101</v>
+      </c>
+      <c r="I10" t="s">
+        <v>44</v>
+      </c>
+      <c r="J10" t="s">
+        <v>109</v>
+      </c>
+      <c r="K10" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" t="s">
+        <v>95</v>
+      </c>
+      <c r="C11" t="s">
+        <v>96</v>
+      </c>
+      <c r="E11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" t="s">
+        <v>102</v>
+      </c>
+      <c r="G11" t="s">
+        <v>103</v>
+      </c>
+      <c r="I11" t="s">
+        <v>48</v>
+      </c>
+      <c r="J11" t="s">
+        <v>111</v>
+      </c>
+      <c r="K11" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" t="s">
+        <v>104</v>
+      </c>
+      <c r="C12" t="s">
+        <v>113</v>
+      </c>
+      <c r="E12" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" t="s">
+        <v>122</v>
+      </c>
+      <c r="G12" t="s">
+        <v>123</v>
+      </c>
+      <c r="I12" t="s">
+        <v>45</v>
+      </c>
+      <c r="J12" t="s">
+        <v>130</v>
+      </c>
+      <c r="K12" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" t="s">
+        <v>114</v>
+      </c>
+      <c r="C13" t="s">
+        <v>115</v>
+      </c>
+      <c r="E13" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" t="s">
+        <v>120</v>
+      </c>
+      <c r="G13" t="s">
+        <v>121</v>
+      </c>
+      <c r="I13" t="s">
+        <v>46</v>
+      </c>
+      <c r="J13" t="s">
+        <v>114</v>
+      </c>
+      <c r="K13" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" t="s">
+        <v>116</v>
+      </c>
+      <c r="C14" t="s">
+        <v>117</v>
+      </c>
+      <c r="E14" t="s">
+        <v>52</v>
+      </c>
+      <c r="F14" t="s">
+        <v>124</v>
+      </c>
+      <c r="G14" t="s">
+        <v>125</v>
+      </c>
+      <c r="I14" t="s">
+        <v>52</v>
+      </c>
+      <c r="J14" t="s">
+        <v>128</v>
+      </c>
+      <c r="K14" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" t="s">
+        <v>118</v>
+      </c>
+      <c r="C15" t="s">
+        <v>119</v>
+      </c>
+      <c r="E15" t="s">
+        <v>49</v>
+      </c>
+      <c r="F15" t="s">
+        <v>126</v>
+      </c>
+      <c r="G15" t="s">
+        <v>127</v>
+      </c>
+      <c r="I15" t="s">
+        <v>49</v>
+      </c>
+      <c r="J15" t="s">
+        <v>132</v>
+      </c>
+      <c r="K15" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" t="s">
+        <v>134</v>
+      </c>
+      <c r="C16" t="s">
+        <v>135</v>
+      </c>
       <c r="E16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F16" t="s">
         <v>142</v>
@@ -1911,19 +2646,25 @@
         <v>143</v>
       </c>
       <c r="I16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J16" t="s">
-        <v>133</v>
+        <v>150</v>
       </c>
       <c r="K16" t="s">
-        <v>134</v>
+        <v>151</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>53</v>
       </c>
+      <c r="B17" t="s">
+        <v>136</v>
+      </c>
+      <c r="C17" t="s">
+        <v>137</v>
+      </c>
       <c r="E17" t="s">
         <v>53</v>
       </c>
@@ -1937,54 +2678,126 @@
         <v>53</v>
       </c>
       <c r="J17" t="s">
-        <v>68</v>
+        <v>152</v>
       </c>
       <c r="K17" t="s">
-        <v>137</v>
+        <v>153</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+      <c r="A18" t="s">
         <v>54</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="B18" t="s">
+        <v>138</v>
+      </c>
+      <c r="C18" t="s">
+        <v>139</v>
+      </c>
+      <c r="E18" t="s">
         <v>54</v>
       </c>
-      <c r="I18" s="3" t="s">
+      <c r="F18" t="s">
+        <v>146</v>
+      </c>
+      <c r="G18" t="s">
+        <v>147</v>
+      </c>
+      <c r="I18" t="s">
         <v>54</v>
       </c>
+      <c r="J18" t="s">
+        <v>154</v>
+      </c>
+      <c r="K18" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="A19" t="s">
         <v>55</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="B19" t="s">
+        <v>140</v>
+      </c>
+      <c r="C19" t="s">
+        <v>141</v>
+      </c>
+      <c r="E19" t="s">
         <v>55</v>
       </c>
-      <c r="I19" s="3" t="s">
+      <c r="F19" t="s">
+        <v>148</v>
+      </c>
+      <c r="G19" t="s">
+        <v>149</v>
+      </c>
+      <c r="I19" t="s">
         <v>55</v>
+      </c>
+      <c r="J19" t="s">
+        <v>156</v>
+      </c>
+      <c r="K19" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>56</v>
       </c>
+      <c r="B20" t="s">
+        <v>158</v>
+      </c>
+      <c r="C20" t="s">
+        <v>159</v>
+      </c>
       <c r="E20" t="s">
         <v>56</v>
       </c>
+      <c r="F20" t="s">
+        <v>162</v>
+      </c>
+      <c r="G20" t="s">
+        <v>163</v>
+      </c>
       <c r="I20" t="s">
         <v>56</v>
+      </c>
+      <c r="J20" t="s">
+        <v>166</v>
+      </c>
+      <c r="K20" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>57</v>
       </c>
+      <c r="B21" t="s">
+        <v>160</v>
+      </c>
+      <c r="C21" t="s">
+        <v>161</v>
+      </c>
       <c r="E21" t="s">
         <v>57</v>
       </c>
+      <c r="F21" t="s">
+        <v>164</v>
+      </c>
+      <c r="G21" t="s">
+        <v>165</v>
+      </c>
       <c r="I21" t="s">
         <v>57</v>
+      </c>
+      <c r="J21" t="s">
+        <v>168</v>
+      </c>
+      <c r="K21" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -1992,28 +2805,22 @@
         <v>58</v>
       </c>
       <c r="B22" t="s">
-        <v>71</v>
+        <v>170</v>
       </c>
       <c r="C22" t="s">
-        <v>72</v>
+        <v>171</v>
       </c>
       <c r="E22" t="s">
         <v>58</v>
       </c>
-      <c r="F22" t="s">
-        <v>107</v>
-      </c>
-      <c r="G22" t="s">
-        <v>106</v>
-      </c>
       <c r="I22" t="s">
         <v>58</v>
       </c>
       <c r="J22" t="s">
-        <v>71</v>
+        <v>170</v>
       </c>
       <c r="K22" t="s">
-        <v>72</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added iteration for features, stride to 0.01 mfcc
</commit_message>
<xml_diff>
--- a/logs/recap risultati.xlsx
+++ b/logs/recap risultati.xlsx
@@ -8,16 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mp95\PycharmProjects\Thesis\logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{88D04BB0-1371-43F3-A89E-BE76FC451DD6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8677A5F0-7DBE-46B0-B66C-9599C16903FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3660" yWindow="285" windowWidth="24930" windowHeight="15195" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2910" yWindow="0" windowWidth="24930" windowHeight="15195" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
     <sheet name="google colab" sheetId="2" r:id="rId2"/>
     <sheet name="setseed5k" sheetId="3" r:id="rId3"/>
     <sheet name="setseed10k" sheetId="4" r:id="rId4"/>
+    <sheet name="colabchoosen10k" sheetId="5" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">setseed10k!$E$3:$G$22</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="157">
   <si>
     <t>LOSS</t>
   </si>
@@ -247,313 +251,314 @@
     <t>NO DROPOUT LAST LAYER</t>
   </si>
   <si>
-    <t>0.7590017914772034</t>
-  </si>
-  <si>
-    <t>0.05325890896519597</t>
-  </si>
-  <si>
-    <t>0.7020499110221863</t>
-  </si>
-  <si>
-    <t>0.08021296184752935</t>
-  </si>
-  <si>
-    <t>0.7322638213634491</t>
-  </si>
-  <si>
-    <t>0.07093958903319733</t>
-  </si>
-  <si>
-    <t>0.7085561573505401</t>
-  </si>
-  <si>
-    <t>0.06344033394508111</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.6787878781557083  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.10935882783927549  </t>
-  </si>
-  <si>
-    <t>0.759090918302536</t>
-  </si>
-  <si>
-    <t>0.06358173387784516</t>
-  </si>
-  <si>
-    <t>0.746880578994751</t>
-  </si>
-  <si>
-    <t>0.07654824535673742</t>
-  </si>
-  <si>
-    <t>0.7262032091617584</t>
-  </si>
-  <si>
-    <t>0.05915319035203717</t>
-  </si>
-  <si>
-    <t>0.7348484754562378</t>
-  </si>
-  <si>
-    <t>0.06652358182743892</t>
-  </si>
-  <si>
-    <t>0.7649732649326324</t>
-  </si>
-  <si>
-    <t>0.04590329043710351</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.7352049887180329  </t>
-  </si>
-  <si>
-    <t>0.06336823291250288</t>
-  </si>
-  <si>
-    <t>0.762210339307785</t>
-  </si>
-  <si>
-    <t>0.07008408082386218</t>
-  </si>
-  <si>
-    <t>0.7501782596111297</t>
-  </si>
-  <si>
-    <t>0.04518646133903952</t>
-  </si>
-  <si>
-    <t>0.7681818187236786</t>
-  </si>
-  <si>
-    <t>0.051071077961338134</t>
-  </si>
-  <si>
-    <t>0.770944744348526</t>
-  </si>
-  <si>
-    <t>0.06314036835574521</t>
-  </si>
-  <si>
-    <t>0.061751001453896906</t>
-  </si>
-  <si>
-    <t>0.7737967908382416</t>
-  </si>
-  <si>
-    <t>0.042515891167034074</t>
-  </si>
-  <si>
-    <t>0.7708556115627289</t>
-  </si>
-  <si>
-    <t>0.09932510215261818</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.7619429588317871  </t>
-  </si>
-  <si>
-    <t>0.7737967848777771</t>
-  </si>
-  <si>
-    <t>0.057730063506272536</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.7474153339862823  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.07631564834152099  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.7679144442081451  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.05218920974581887  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.7677361845970154  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.06601287893824767  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.025823484551640637  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.7766488373279572  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.031395325500609604  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.7500891268253327  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.05590899343192252  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.7381461679935455  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.06122001467009059  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.7441176474094391  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0526291418700324  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.7559714794158936  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.046944909503834946  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.7769162237644196  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.04375206233526736  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.7737967908382416  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.03795116810290435  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.7799465298652649  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.07081771633972618  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.7676470637321472  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.04047965276517804  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.7679144382476807  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.04695404745223683  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.7648841440677643  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.03825761552653673  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.7706773757934571  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.05014594711373972  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.7768270969390869  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.04195239738352049  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.7975044548511505  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.04595819948864746  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.7857397556304931  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.04729790924985195  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.7827094554901123  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0324518693567599  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.7855614960193634  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.04971983875716206  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.7945632755756378  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.049141394508279125  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.7796791553497314  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.04042416732337842  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.7826203286647797  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.040691819639471216  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.7707664906978607  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0402646941606926  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.7884135544300079  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.03992073781479127  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.7499108791351319  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.04467579656291825  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.7675579369068146  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.053641751623085494  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.758734405040741  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.047598997655352665  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.7796791434288025  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.04834045464414888  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.7380570352077485  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.037007269917630786  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.7707664966583252  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.050287915764755546  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.7500000059604645  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.04596070609500026  </t>
+    <t>Accuracy std, dev</t>
+  </si>
+  <si>
+    <t>0.756648844242096</t>
+  </si>
+  <si>
+    <t>0.06185563637322689</t>
+  </si>
+  <si>
+    <t>0.015460310648409503</t>
+  </si>
+  <si>
+    <t>0.010983530702245944</t>
+  </si>
+  <si>
+    <t>0.2068627381324768</t>
+  </si>
+  <si>
+    <t>0.7717985768318176</t>
+  </si>
+  <si>
+    <t>0.011213156080405975</t>
+  </si>
+  <si>
+    <t>0.05800422953446706</t>
+  </si>
+  <si>
+    <t>0.012127206439949419</t>
+  </si>
+  <si>
+    <t>0.18994651794433592</t>
+  </si>
+  <si>
+    <t>0.76498752450943</t>
+  </si>
+  <si>
+    <t>0.060148136071229714</t>
+  </si>
+  <si>
+    <t>0.009151579506043152</t>
+  </si>
+  <si>
+    <t>0.013519363128241979</t>
+  </si>
+  <si>
+    <t>0.19909090042114258</t>
+  </si>
+  <si>
+    <t>0.0467121476180913</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7667789680957795  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.012597815183029796  </t>
+  </si>
+  <si>
+    <t>0.010786699964569182</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.19327984809875487  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.04529734209167729  </t>
+  </si>
+  <si>
+    <t>Time elapsed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7618181852102279  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.06270180865319902  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.015154197816941488  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.017195654019701714 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.2093582797050476  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.05671454244369726  </t>
+  </si>
+  <si>
+    <t>0.7682549037933348</t>
+  </si>
+  <si>
+    <t>0.010052680260276094</t>
+  </si>
+  <si>
+    <t>0.06017383464855589</t>
+  </si>
+  <si>
+    <t>0.016129846154919903</t>
+  </si>
+  <si>
+    <t>0.19459892749786378</t>
+  </si>
+  <si>
+    <t>0.05338632012955206</t>
+  </si>
+  <si>
+    <t>0.05643172257620497</t>
+  </si>
+  <si>
+    <t>0.7726221054792406</t>
+  </si>
+  <si>
+    <t>0.0606260657675694</t>
+  </si>
+  <si>
+    <t>0.014169548589983039</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.010512895193503456</t>
+  </si>
+  <si>
+    <t>0.2032620346546173</t>
+  </si>
+  <si>
+    <t>0.054206944598473486</t>
+  </si>
+  <si>
+    <t>0.7506167578697205</t>
+  </si>
+  <si>
+    <t>0.06371269097093112</t>
+  </si>
+  <si>
+    <t>0.014023002273968112</t>
+  </si>
+  <si>
+    <t>0.0148338714061927</t>
+  </si>
+  <si>
+    <t>0.21263814091682434</t>
+  </si>
+  <si>
+    <t>0.05273463403554979</t>
+  </si>
+  <si>
+    <t>0.7725205019712449</t>
+  </si>
+  <si>
+    <t>0.06353944667878769</t>
+  </si>
+  <si>
+    <t>0.010855753075669784</t>
+  </si>
+  <si>
+    <t>0.01502501085299153</t>
+  </si>
+  <si>
+    <t>0.213493754863739</t>
+  </si>
+  <si>
+    <t>0.056251560121431995</t>
+  </si>
+  <si>
+    <t>0.7640142626762391</t>
+  </si>
+  <si>
+    <t>0.06322673600043721</t>
+  </si>
+  <si>
+    <t>0.01418897548232081</t>
+  </si>
+  <si>
+    <t>0.011102830765937299</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.21115864276885987 </t>
+  </si>
+  <si>
+    <t>0.05724585745675555</t>
+  </si>
+  <si>
+    <t>NO DROPOUT</t>
+  </si>
+  <si>
+    <t>FULL DROPOUT</t>
+  </si>
+  <si>
+    <t>LAST DROPOUT</t>
+  </si>
+  <si>
+    <t>0.7707130146026612</t>
+  </si>
+  <si>
+    <t>0.06048648266063122</t>
+  </si>
+  <si>
+    <t>0.013815398143398471</t>
+  </si>
+  <si>
+    <t>0.012760968489824694</t>
+  </si>
+  <si>
+    <t>0.20057040572166443</t>
+  </si>
+  <si>
+    <t>0.050880868400958804</t>
+  </si>
+  <si>
+    <t>LSTM(256)
+LSTM(128)</t>
+  </si>
+  <si>
+    <t>LSTM(128)
+LSTM(64)
+Dense (64)</t>
+  </si>
+  <si>
+    <t>LSTM(256) 
+LSTM(128)
+Dense(64)</t>
+  </si>
+  <si>
+    <t>LSTM(256)
+Dropout(0.5)
+LSTM(128)
+Dropout(0.5)
+Dense(64)
+Dropout(0.5)</t>
+  </si>
+  <si>
+    <t>LSTM(256) 
+Dropout(0.5)
+Dense(64)
+Dropout(0.5)</t>
+  </si>
+  <si>
+    <t>LSTM(256)
+Dropout(0.5)
+LSTM(128)
+Dropout(0.5)</t>
+  </si>
+  <si>
+    <t>LSTM(256)
+Dropout(0.5)
+LSTM(128)
+Dropout(0.5)
+LSTM(64)
+Dropout(0.5)
+dense(32)
+Dropout(0.5)</t>
+  </si>
+  <si>
+    <t>LSTM(256)
+Dropout(0.5)
+LSTM(128) 
+Dropout(0.5)
+Dense(64)</t>
+  </si>
+  <si>
+    <t>LSTM(256)
+Dropout(0.5)
+LSTM(128)</t>
+  </si>
+  <si>
+    <t>LSTM(256)
+Dropout(0.5)
+Dense(256)
+Dropout(0.5)</t>
+  </si>
+  <si>
+    <t>LSTM(256)
+Dropout(0.5)
+Dense(64)
+Dropout(0.5)</t>
+  </si>
+  <si>
+    <t>0.049</t>
+  </si>
+  <si>
+    <t>0.056</t>
+  </si>
+  <si>
+    <t>Average Accuracy Std.Dev between folders
+across  iterations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average Accuracy 
+between folders
+across iterations </t>
+  </si>
+  <si>
+    <t>Average Std.Dev of 
+the average accuracy
+across iterations</t>
+  </si>
+  <si>
+    <t>Average Std. Dev of
+the average accuracy Std.Dev
+across  iterations</t>
+  </si>
+  <si>
+    <t>Average max-min accuracy 
+difference between folders 
+across iterations</t>
+  </si>
+  <si>
+    <t>max-min accuracy difference
+ Std.Dev between folders
+across iterations</t>
   </si>
 </sst>
 </file>
@@ -572,7 +577,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -582,6 +587,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -598,7 +609,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -612,6 +623,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -620,6 +632,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -916,7 +935,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>7</v>
       </c>
       <c r="C1" t="s">
@@ -931,7 +950,7 @@
       <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="10" t="s">
         <v>9</v>
       </c>
       <c r="J1" t="s">
@@ -948,7 +967,7 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
+      <c r="A2" s="11"/>
       <c r="B2" t="s">
         <v>4</v>
       </c>
@@ -964,7 +983,7 @@
       <c r="F2">
         <v>0.02</v>
       </c>
-      <c r="H2" s="9"/>
+      <c r="H2" s="10"/>
       <c r="I2" t="s">
         <v>16</v>
       </c>
@@ -982,7 +1001,7 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
+      <c r="A3" s="11"/>
       <c r="B3" t="s">
         <v>5</v>
       </c>
@@ -998,7 +1017,7 @@
       <c r="F3">
         <v>0.04</v>
       </c>
-      <c r="H3" s="9"/>
+      <c r="H3" s="10"/>
       <c r="I3" t="s">
         <v>17</v>
       </c>
@@ -1010,7 +1029,7 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="10"/>
+      <c r="A4" s="11"/>
       <c r="B4" t="s">
         <v>6</v>
       </c>
@@ -1026,7 +1045,7 @@
       <c r="F4">
         <v>0.01</v>
       </c>
-      <c r="H4" s="9"/>
+      <c r="H4" s="10"/>
       <c r="I4" t="s">
         <v>18</v>
       </c>
@@ -1038,7 +1057,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H5" s="9"/>
+      <c r="H5" s="10"/>
       <c r="I5" t="s">
         <v>20</v>
       </c>
@@ -1053,7 +1072,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H6" s="9"/>
+      <c r="H6" s="10"/>
       <c r="I6" t="s">
         <v>19</v>
       </c>
@@ -1068,7 +1087,7 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H7" s="9"/>
+      <c r="H7" s="10"/>
       <c r="I7" t="s">
         <v>10</v>
       </c>
@@ -1086,7 +1105,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H8" s="9"/>
+      <c r="H8" s="10"/>
       <c r="I8" t="s">
         <v>11</v>
       </c>
@@ -1104,7 +1123,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H9" s="9"/>
+      <c r="H9" s="10"/>
       <c r="I9" t="s">
         <v>12</v>
       </c>
@@ -1125,7 +1144,7 @@
       <c r="B10" t="s">
         <v>8</v>
       </c>
-      <c r="H10" s="9"/>
+      <c r="H10" s="10"/>
       <c r="I10" t="s">
         <v>13</v>
       </c>
@@ -1143,7 +1162,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H11" s="9"/>
+      <c r="H11" s="10"/>
       <c r="I11" t="s">
         <v>14</v>
       </c>
@@ -1161,7 +1180,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H12" s="9"/>
+      <c r="H12" s="10"/>
       <c r="I12" t="s">
         <v>15</v>
       </c>
@@ -1179,7 +1198,7 @@
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H13" s="9"/>
+      <c r="H13" s="10"/>
       <c r="I13" t="s">
         <v>21</v>
       </c>
@@ -1197,7 +1216,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H14" s="9"/>
+      <c r="H14" s="10"/>
       <c r="I14" t="s">
         <v>15</v>
       </c>
@@ -1215,7 +1234,7 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H15" s="9"/>
+      <c r="H15" s="10"/>
       <c r="I15" t="s">
         <v>22</v>
       </c>
@@ -1233,7 +1252,7 @@
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H16" s="9"/>
+      <c r="H16" s="10"/>
       <c r="I16" t="s">
         <v>34</v>
       </c>
@@ -1251,7 +1270,7 @@
       </c>
     </row>
     <row r="17" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H17" s="9"/>
+      <c r="H17" s="10"/>
       <c r="I17" t="s">
         <v>37</v>
       </c>
@@ -1260,13 +1279,13 @@
       </c>
     </row>
     <row r="18" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H18" s="9"/>
+      <c r="H18" s="10"/>
     </row>
     <row r="19" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H19" s="9"/>
+      <c r="H19" s="10"/>
     </row>
     <row r="20" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H20" s="9"/>
+      <c r="H20" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1590,21 +1609,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="E1" s="11" t="s">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="E1" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="I1" s="11" t="s">
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="I1" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
@@ -2220,10 +2239,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BED2715A-8FB0-46CE-8864-89EDF7D1B731}">
-  <dimension ref="A1:K22"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:C22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2240,21 +2259,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="E1" s="11" t="s">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="E1" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="I1" s="11" t="s">
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="I1" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
@@ -2268,562 +2287,637 @@
       <c r="K2" s="8"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E3" t="s">
+      <c r="B3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I3" t="s">
+      <c r="F3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2" t="s">
         <v>40</v>
       </c>
+      <c r="J3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="4">
+        <v>0.79750445485114996</v>
+      </c>
+      <c r="C4" s="4">
+        <v>4.5958199488647399E-2</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0.794563275575637</v>
+      </c>
+      <c r="G4" s="4">
+        <v>4.9141394508279097E-2</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J4" s="4">
+        <v>0.78841355443000705</v>
+      </c>
+      <c r="K4" s="4">
+        <v>3.9920737814791198E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.77682709693908603</v>
+      </c>
+      <c r="C5" s="2">
+        <v>4.1952397383520398E-2</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0.78573975563049303</v>
+      </c>
+      <c r="G5" s="4">
+        <v>4.7297909249851902E-2</v>
+      </c>
+      <c r="H5" s="2"/>
+      <c r="I5" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="J5" s="4">
+        <v>0.78262032866477904</v>
+      </c>
+      <c r="K5" s="4">
+        <v>4.0691819639471202E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="4">
+        <v>0.77664883732795698</v>
+      </c>
+      <c r="C6" s="4">
+        <v>3.1395325500609597E-2</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.78556149601936298</v>
+      </c>
+      <c r="G6" s="2">
+        <v>4.9719838757162002E-2</v>
+      </c>
+      <c r="H6" s="2"/>
+      <c r="I6" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="J6" s="4">
+        <v>0.77994652986526403</v>
+      </c>
+      <c r="K6" s="4">
+        <v>7.0817716339726097E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="4">
+        <v>0.77067737579345696</v>
+      </c>
+      <c r="C7" s="4">
+        <v>5.0145947113739701E-2</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F7" s="4">
+        <v>0.78270945549011195</v>
+      </c>
+      <c r="G7" s="4">
+        <v>3.2451869356759901E-2</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J7" s="4">
+        <v>0.77967915534973098</v>
+      </c>
+      <c r="K7" s="4">
+        <v>4.0424167323378397E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="9">
+        <v>0.76818181872367797</v>
+      </c>
+      <c r="C8" s="9">
+        <v>5.1071077961338099E-2</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F8" s="9">
+        <v>0.77967914342880196</v>
+      </c>
+      <c r="G8" s="9">
+        <v>4.8340454644148802E-2</v>
+      </c>
+      <c r="H8" s="2"/>
+      <c r="I8" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="J8" s="4">
+        <v>0.77664883732795698</v>
+      </c>
+      <c r="K8" s="4">
+        <v>3.1395325500609597E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0.76755793690681395</v>
+      </c>
+      <c r="C9" s="2">
+        <v>5.3641751623085397E-2</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0.77691622376441904</v>
+      </c>
+      <c r="G9" s="2">
+        <v>4.3752062335267301E-2</v>
+      </c>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="J9" s="2">
+        <v>0.77379678487777703</v>
+      </c>
+      <c r="K9" s="2">
+        <v>5.7730063506272501E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0.76488414406776395</v>
+      </c>
+      <c r="C10" s="2">
+        <v>3.8257615526536698E-2</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0.77379679083824104</v>
+      </c>
+      <c r="G10" s="2">
+        <v>4.2515891167033998E-2</v>
+      </c>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="J10" s="2">
+        <v>0.77076649665832497</v>
+      </c>
+      <c r="K10" s="2">
+        <v>5.0287915764755498E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="2">
+        <v>0.76221033930778503</v>
+      </c>
+      <c r="C11" s="2">
+        <v>7.0084080823862097E-2</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0.77379679083824104</v>
+      </c>
+      <c r="G11" s="2">
+        <v>3.7951168102904297E-2</v>
+      </c>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="J11" s="2">
+        <v>0.77076649069785996</v>
+      </c>
+      <c r="K11" s="2">
+        <v>4.0264694160692602E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="2">
+        <v>0.76194295883178698</v>
+      </c>
+      <c r="C12" s="2">
+        <v>2.5823484551640598E-2</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="2">
+        <v>0.770944744348526</v>
+      </c>
+      <c r="G12" s="2">
+        <v>6.3140368355745199E-2</v>
+      </c>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J12" s="2">
+        <v>0.76791444420814503</v>
+      </c>
+      <c r="K12" s="2">
+        <v>5.2189209745818803E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="2">
+        <v>0.75900179147720304</v>
+      </c>
+      <c r="C13" s="2">
+        <v>5.3258908965195903E-2</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F13" s="2">
+        <v>0.77085561156272797</v>
+      </c>
+      <c r="G13" s="2">
+        <v>9.9325102152618097E-2</v>
+      </c>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="J13" s="2">
+        <v>0.76791443824768002</v>
+      </c>
+      <c r="K13" s="2">
+        <v>4.6954047452236802E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="2">
+        <v>0.75017825961112905</v>
+      </c>
+      <c r="C14" s="2">
+        <v>4.5186461339039502E-2</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" s="2">
+        <v>0.75909091830253606</v>
+      </c>
+      <c r="G14" s="2">
+        <v>6.3581733877845104E-2</v>
+      </c>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="J14" s="2">
+        <v>0.76773618459701498</v>
+      </c>
+      <c r="K14" s="2">
+        <v>6.6012878938247602E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" s="2">
+        <v>0.75008912682533202</v>
+      </c>
+      <c r="C15" s="2">
+        <v>5.5908993431922502E-2</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F15" s="2">
+        <v>0.75873440504074097</v>
+      </c>
+      <c r="G15" s="2">
+        <v>4.7598997655352603E-2</v>
+      </c>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J15" s="2">
+        <v>0.76764706373214697</v>
+      </c>
+      <c r="K15" s="2">
+        <v>4.0479652765178002E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" s="2">
+        <v>0.75000000596046401</v>
+      </c>
+      <c r="C16" s="2">
+        <v>4.5960706095000199E-2</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" s="2">
+        <v>0.75597147941589304</v>
+      </c>
+      <c r="G16" s="2">
+        <v>4.6944909503834897E-2</v>
+      </c>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="J16" s="2">
+        <v>0.76497326493263196</v>
+      </c>
+      <c r="K16" s="2">
+        <v>4.5903290437103499E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" s="2">
+        <v>0.74991087913513099</v>
+      </c>
+      <c r="C17" s="2">
+        <v>4.4675796562918202E-2</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F17" s="2">
+        <v>0.75311943888664201</v>
+      </c>
+      <c r="G17" s="2">
+        <v>4.5196922589280999E-2</v>
+      </c>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J17" s="2">
+        <v>0.75900179147720304</v>
+      </c>
+      <c r="K17" s="2">
+        <v>5.3258908965195903E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" s="2">
+        <v>0.73814616799354504</v>
+      </c>
+      <c r="C18" s="2">
+        <v>6.12200146700905E-2</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F18" s="2">
+        <v>0.74688057899475102</v>
+      </c>
+      <c r="G18" s="2">
+        <v>7.6548245356737404E-2</v>
+      </c>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="J18" s="2">
+        <v>0.75000000596046401</v>
+      </c>
+      <c r="K18" s="2">
+        <v>4.5960706095000199E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" s="2">
+        <v>0.73520498871803197</v>
+      </c>
+      <c r="C19" s="2">
+        <v>6.3368232912502806E-2</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F19" s="2">
+        <v>0.74411764740943898</v>
+      </c>
+      <c r="G19" s="2">
+        <v>5.2629141870032398E-2</v>
+      </c>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="J19" s="2">
+        <v>0.74741533398628202</v>
+      </c>
+      <c r="K19" s="2">
+        <v>7.6315648341520895E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="2">
+        <v>0.73226382136344903</v>
+      </c>
+      <c r="C20" s="2">
+        <v>7.0939589033197303E-2</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F20" s="2">
+        <v>0.72620320916175796</v>
+      </c>
+      <c r="G20" s="2">
+        <v>5.9153190352037102E-2</v>
+      </c>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="J20" s="2">
+        <v>0.73805703520774801</v>
+      </c>
+      <c r="K20" s="2">
+        <v>3.7007269917630703E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="2">
+        <v>0.70855615735054001</v>
+      </c>
+      <c r="C21" s="2">
+        <v>6.3440333945081098E-2</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F21" s="2">
+        <v>0.72620320916175796</v>
+      </c>
+      <c r="G21" s="2">
+        <v>6.1751001453896899E-2</v>
+      </c>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J21" s="2">
+        <v>0.73484847545623699</v>
+      </c>
+      <c r="K21" s="2">
+        <v>6.6523581827438893E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B4" t="s">
-        <v>71</v>
-      </c>
-      <c r="C4" t="s">
-        <v>72</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="B22" s="2">
+        <v>0.70204991102218595</v>
+      </c>
+      <c r="C22" s="2">
+        <v>8.0212961847529296E-2</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="F4" t="s">
-        <v>77</v>
-      </c>
-      <c r="G4" t="s">
-        <v>78</v>
-      </c>
-      <c r="I4" t="s">
+      <c r="F22" s="2">
+        <v>0.67878787815570796</v>
+      </c>
+      <c r="G22" s="2">
+        <v>0.109358827839275</v>
+      </c>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="J4" t="s">
-        <v>71</v>
-      </c>
-      <c r="K4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C5" t="s">
-        <v>70</v>
-      </c>
-      <c r="E5" t="s">
-        <v>41</v>
-      </c>
-      <c r="F5" t="s">
-        <v>79</v>
-      </c>
-      <c r="G5" t="s">
-        <v>80</v>
-      </c>
-      <c r="I5" t="s">
-        <v>41</v>
-      </c>
-      <c r="J5" t="s">
-        <v>69</v>
-      </c>
-      <c r="K5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B6" t="s">
-        <v>73</v>
-      </c>
-      <c r="C6" t="s">
-        <v>74</v>
-      </c>
-      <c r="E6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F6" t="s">
-        <v>81</v>
-      </c>
-      <c r="G6" t="s">
-        <v>82</v>
-      </c>
-      <c r="I6" t="s">
-        <v>42</v>
-      </c>
-      <c r="J6" t="s">
-        <v>85</v>
-      </c>
-      <c r="K6" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>47</v>
-      </c>
-      <c r="B7" t="s">
-        <v>75</v>
-      </c>
-      <c r="C7" t="s">
-        <v>76</v>
-      </c>
-      <c r="E7" t="s">
-        <v>47</v>
-      </c>
-      <c r="F7" t="s">
-        <v>83</v>
-      </c>
-      <c r="G7" t="s">
-        <v>84</v>
-      </c>
-      <c r="I7" t="s">
-        <v>47</v>
-      </c>
-      <c r="J7" t="s">
-        <v>87</v>
-      </c>
-      <c r="K7" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>59</v>
-      </c>
-      <c r="B8" t="s">
-        <v>89</v>
-      </c>
-      <c r="C8" t="s">
-        <v>90</v>
-      </c>
-      <c r="E8" t="s">
-        <v>59</v>
-      </c>
-      <c r="F8" t="s">
-        <v>83</v>
-      </c>
-      <c r="G8" t="s">
-        <v>99</v>
-      </c>
-      <c r="I8" t="s">
-        <v>59</v>
-      </c>
-      <c r="J8" t="s">
-        <v>107</v>
-      </c>
-      <c r="K8" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B9" t="s">
-        <v>91</v>
-      </c>
-      <c r="C9" t="s">
-        <v>92</v>
-      </c>
-      <c r="E9" t="s">
-        <v>43</v>
-      </c>
-      <c r="F9" t="s">
-        <v>97</v>
-      </c>
-      <c r="G9" t="s">
-        <v>98</v>
-      </c>
-      <c r="I9" t="s">
-        <v>43</v>
-      </c>
-      <c r="J9" t="s">
-        <v>105</v>
-      </c>
-      <c r="K9" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>44</v>
-      </c>
-      <c r="B10" t="s">
-        <v>93</v>
-      </c>
-      <c r="C10" t="s">
-        <v>94</v>
-      </c>
-      <c r="E10" t="s">
-        <v>44</v>
-      </c>
-      <c r="F10" t="s">
-        <v>100</v>
-      </c>
-      <c r="G10" t="s">
-        <v>101</v>
-      </c>
-      <c r="I10" t="s">
-        <v>44</v>
-      </c>
-      <c r="J10" t="s">
-        <v>109</v>
-      </c>
-      <c r="K10" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>48</v>
-      </c>
-      <c r="B11" t="s">
-        <v>95</v>
-      </c>
-      <c r="C11" t="s">
-        <v>96</v>
-      </c>
-      <c r="E11" t="s">
-        <v>48</v>
-      </c>
-      <c r="F11" t="s">
-        <v>102</v>
-      </c>
-      <c r="G11" t="s">
-        <v>103</v>
-      </c>
-      <c r="I11" t="s">
-        <v>48</v>
-      </c>
-      <c r="J11" t="s">
-        <v>111</v>
-      </c>
-      <c r="K11" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>45</v>
-      </c>
-      <c r="B12" t="s">
-        <v>104</v>
-      </c>
-      <c r="C12" t="s">
-        <v>113</v>
-      </c>
-      <c r="E12" t="s">
-        <v>45</v>
-      </c>
-      <c r="F12" t="s">
-        <v>122</v>
-      </c>
-      <c r="G12" t="s">
-        <v>123</v>
-      </c>
-      <c r="I12" t="s">
-        <v>45</v>
-      </c>
-      <c r="J12" t="s">
-        <v>130</v>
-      </c>
-      <c r="K12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>46</v>
-      </c>
-      <c r="B13" t="s">
-        <v>114</v>
-      </c>
-      <c r="C13" t="s">
-        <v>115</v>
-      </c>
-      <c r="E13" t="s">
-        <v>46</v>
-      </c>
-      <c r="F13" t="s">
-        <v>120</v>
-      </c>
-      <c r="G13" t="s">
-        <v>121</v>
-      </c>
-      <c r="I13" t="s">
-        <v>46</v>
-      </c>
-      <c r="J13" t="s">
-        <v>114</v>
-      </c>
-      <c r="K13" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>52</v>
-      </c>
-      <c r="B14" t="s">
-        <v>116</v>
-      </c>
-      <c r="C14" t="s">
-        <v>117</v>
-      </c>
-      <c r="E14" t="s">
-        <v>52</v>
-      </c>
-      <c r="F14" t="s">
-        <v>124</v>
-      </c>
-      <c r="G14" t="s">
-        <v>125</v>
-      </c>
-      <c r="I14" t="s">
-        <v>52</v>
-      </c>
-      <c r="J14" t="s">
-        <v>128</v>
-      </c>
-      <c r="K14" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>49</v>
-      </c>
-      <c r="B15" t="s">
-        <v>118</v>
-      </c>
-      <c r="C15" t="s">
-        <v>119</v>
-      </c>
-      <c r="E15" t="s">
-        <v>49</v>
-      </c>
-      <c r="F15" t="s">
-        <v>126</v>
-      </c>
-      <c r="G15" t="s">
-        <v>127</v>
-      </c>
-      <c r="I15" t="s">
-        <v>49</v>
-      </c>
-      <c r="J15" t="s">
-        <v>132</v>
-      </c>
-      <c r="K15" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B16" t="s">
-        <v>134</v>
-      </c>
-      <c r="C16" t="s">
-        <v>135</v>
-      </c>
-      <c r="E16" t="s">
-        <v>50</v>
-      </c>
-      <c r="F16" t="s">
-        <v>142</v>
-      </c>
-      <c r="G16" t="s">
-        <v>143</v>
-      </c>
-      <c r="I16" t="s">
-        <v>50</v>
-      </c>
-      <c r="J16" t="s">
-        <v>150</v>
-      </c>
-      <c r="K16" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>53</v>
-      </c>
-      <c r="B17" t="s">
-        <v>136</v>
-      </c>
-      <c r="C17" t="s">
-        <v>137</v>
-      </c>
-      <c r="E17" t="s">
-        <v>53</v>
-      </c>
-      <c r="F17" t="s">
-        <v>144</v>
-      </c>
-      <c r="G17" t="s">
-        <v>145</v>
-      </c>
-      <c r="I17" t="s">
-        <v>53</v>
-      </c>
-      <c r="J17" t="s">
-        <v>152</v>
-      </c>
-      <c r="K17" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>54</v>
-      </c>
-      <c r="B18" t="s">
-        <v>138</v>
-      </c>
-      <c r="C18" t="s">
-        <v>139</v>
-      </c>
-      <c r="E18" t="s">
-        <v>54</v>
-      </c>
-      <c r="F18" t="s">
-        <v>146</v>
-      </c>
-      <c r="G18" t="s">
-        <v>147</v>
-      </c>
-      <c r="I18" t="s">
-        <v>54</v>
-      </c>
-      <c r="J18" t="s">
-        <v>154</v>
-      </c>
-      <c r="K18" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>55</v>
-      </c>
-      <c r="B19" t="s">
-        <v>140</v>
-      </c>
-      <c r="C19" t="s">
-        <v>141</v>
-      </c>
-      <c r="E19" t="s">
-        <v>55</v>
-      </c>
-      <c r="F19" t="s">
-        <v>148</v>
-      </c>
-      <c r="G19" t="s">
-        <v>149</v>
-      </c>
-      <c r="I19" t="s">
-        <v>55</v>
-      </c>
-      <c r="J19" t="s">
-        <v>156</v>
-      </c>
-      <c r="K19" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>56</v>
-      </c>
-      <c r="B20" t="s">
-        <v>158</v>
-      </c>
-      <c r="C20" t="s">
-        <v>159</v>
-      </c>
-      <c r="E20" t="s">
-        <v>56</v>
-      </c>
-      <c r="F20" t="s">
-        <v>162</v>
-      </c>
-      <c r="G20" t="s">
-        <v>163</v>
-      </c>
-      <c r="I20" t="s">
-        <v>56</v>
-      </c>
-      <c r="J20" t="s">
-        <v>166</v>
-      </c>
-      <c r="K20" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>57</v>
-      </c>
-      <c r="B21" t="s">
-        <v>160</v>
-      </c>
-      <c r="C21" t="s">
-        <v>161</v>
-      </c>
-      <c r="E21" t="s">
-        <v>57</v>
-      </c>
-      <c r="F21" t="s">
-        <v>164</v>
-      </c>
-      <c r="G21" t="s">
-        <v>165</v>
-      </c>
-      <c r="I21" t="s">
-        <v>57</v>
-      </c>
-      <c r="J21" t="s">
-        <v>168</v>
-      </c>
-      <c r="K21" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>58</v>
-      </c>
-      <c r="B22" t="s">
-        <v>170</v>
-      </c>
-      <c r="C22" t="s">
-        <v>171</v>
-      </c>
-      <c r="E22" t="s">
-        <v>58</v>
-      </c>
-      <c r="I22" t="s">
-        <v>58</v>
-      </c>
-      <c r="J22" t="s">
-        <v>170</v>
-      </c>
-      <c r="K22" t="s">
-        <v>171</v>
+      <c r="J22" s="2">
+        <v>0.70204991102218595</v>
+      </c>
+      <c r="K22" s="2">
+        <v>8.0212961847529296E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <f>22-3</f>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="E3:G22" xr:uid="{8399C0EB-58A7-4B5F-B11F-EE40A52248D5}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="E4:G22">
+      <sortCondition descending="1" ref="F3:F22"/>
+    </sortState>
+  </autoFilter>
   <mergeCells count="3">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="E1:G1"/>
@@ -2831,4 +2925,367 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5F52107-7088-41D8-ABD7-D4F6280F9073}">
+  <dimension ref="A1:I13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.28515625" style="13" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H2" t="s">
+        <v>149</v>
+      </c>
+      <c r="I2" s="13">
+        <v>11857</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="14"/>
+      <c r="B3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="I3" s="13">
+        <v>7166</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="14"/>
+      <c r="B4" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="C4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F4" t="s">
+        <v>83</v>
+      </c>
+      <c r="G4" t="s">
+        <v>84</v>
+      </c>
+      <c r="H4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="14"/>
+      <c r="B5" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="C5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D5" t="s">
+        <v>93</v>
+      </c>
+      <c r="E5" t="s">
+        <v>94</v>
+      </c>
+      <c r="F5" t="s">
+        <v>95</v>
+      </c>
+      <c r="G5" t="s">
+        <v>96</v>
+      </c>
+      <c r="H5" t="s">
+        <v>97</v>
+      </c>
+      <c r="I5" s="13">
+        <v>10343</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="C6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D6" t="s">
+        <v>106</v>
+      </c>
+      <c r="E6" t="s">
+        <v>108</v>
+      </c>
+      <c r="F6" t="s">
+        <v>107</v>
+      </c>
+      <c r="G6" t="s">
+        <v>109</v>
+      </c>
+      <c r="H6" t="s">
+        <v>110</v>
+      </c>
+      <c r="I6" s="13">
+        <v>6625</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="14"/>
+      <c r="B7" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="C7" t="s">
+        <v>86</v>
+      </c>
+      <c r="D7" t="s">
+        <v>104</v>
+      </c>
+      <c r="E7" t="s">
+        <v>87</v>
+      </c>
+      <c r="F7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G7" t="s">
+        <v>89</v>
+      </c>
+      <c r="H7" t="s">
+        <v>90</v>
+      </c>
+      <c r="I7">
+        <v>8356</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="14"/>
+      <c r="B8" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="C8" t="s">
+        <v>98</v>
+      </c>
+      <c r="D8" t="s">
+        <v>100</v>
+      </c>
+      <c r="E8" t="s">
+        <v>99</v>
+      </c>
+      <c r="F8" t="s">
+        <v>101</v>
+      </c>
+      <c r="G8" t="s">
+        <v>102</v>
+      </c>
+      <c r="H8" t="s">
+        <v>103</v>
+      </c>
+      <c r="I8" s="13">
+        <v>5688</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+      <c r="A9" s="14"/>
+      <c r="B9" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="C9" t="s">
+        <v>111</v>
+      </c>
+      <c r="D9" t="s">
+        <v>112</v>
+      </c>
+      <c r="E9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F9" t="s">
+        <v>114</v>
+      </c>
+      <c r="G9" t="s">
+        <v>115</v>
+      </c>
+      <c r="H9" t="s">
+        <v>116</v>
+      </c>
+      <c r="I9" s="13">
+        <v>11236</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="C10" t="s">
+        <v>117</v>
+      </c>
+      <c r="D10" t="s">
+        <v>118</v>
+      </c>
+      <c r="E10" t="s">
+        <v>119</v>
+      </c>
+      <c r="F10" t="s">
+        <v>120</v>
+      </c>
+      <c r="G10" t="s">
+        <v>121</v>
+      </c>
+      <c r="H10" t="s">
+        <v>122</v>
+      </c>
+      <c r="I10" s="13">
+        <v>6308</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="14"/>
+      <c r="B11" s="15" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="14"/>
+      <c r="B12" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="C12" t="s">
+        <v>123</v>
+      </c>
+      <c r="D12" t="s">
+        <v>124</v>
+      </c>
+      <c r="E12" t="s">
+        <v>126</v>
+      </c>
+      <c r="F12" t="s">
+        <v>125</v>
+      </c>
+      <c r="G12" t="s">
+        <v>127</v>
+      </c>
+      <c r="H12" t="s">
+        <v>128</v>
+      </c>
+      <c r="I12" s="13">
+        <v>3934</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="14"/>
+      <c r="B13" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="C13" t="s">
+        <v>132</v>
+      </c>
+      <c r="D13" t="s">
+        <v>133</v>
+      </c>
+      <c r="E13" t="s">
+        <v>135</v>
+      </c>
+      <c r="F13" t="s">
+        <v>134</v>
+      </c>
+      <c r="G13" t="s">
+        <v>136</v>
+      </c>
+      <c r="H13" t="s">
+        <v>137</v>
+      </c>
+      <c r="I13" s="13">
+        <v>7774</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="A10:A13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>